<commit_message>
Fix missing lines in S00032
</commit_message>
<xml_diff>
--- a/tl/S00032.MES.BIN.xlsx
+++ b/tl/S00032.MES.BIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B973B3-C6B9-4554-BA73-C439ED58F5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED3BBC8-8E66-46CE-8DDA-84BB6E7E506B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="11310" windowWidth="48240" windowHeight="19545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4815" yWindow="11145" windowWidth="48240" windowHeight="19545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00032.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="401">
   <si>
     <t>Status</t>
   </si>
@@ -68,58 +68,70 @@
     <t>7</t>
   </si>
   <si>
-    <t>Well, I can't say it's not the fault of this special environment.</t>
+    <t>"Echoes"</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>Basically, we create an atmosphere where only regulars can enter.</t>
+    <t>This shop has few customers despite having a special environment where celebrities and those involved in the entertainment industry gather (which is bad for the shop owner).</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
+    <t>Well, I can't deny that it's because of that special environment.</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>In other words, they've created an atmosphere where only regulars can get in.</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>That was a problem when hiring part-timers.</t>
   </si>
   <si>
-    <t>13</t>
+    <t>17</t>
   </si>
   <si>
     <t>Since the regulars are mostly related to the entertainment industry or aspiring entertainers who take lessons every day.</t>
   </si>
   <si>
-    <t>15</t>
+    <t>19</t>
   </si>
   <si>
     <t>...Except for me.</t>
   </si>
   <si>
-    <t>17</t>
+    <t>21</t>
   </si>
   <si>
     <t>They were going to hire a normal part-timer,</t>
   </si>
   <si>
-    <t>19</t>
+    <t>23</t>
   </si>
   <si>
     <t>but at the time of recruitment, it seemed like a bunch of people who obviously came with the intention of meeting a celebrity had shown up.</t>
   </si>
   <si>
-    <t>21</t>
+    <t>25</t>
   </si>
   <si>
     <t>So the store manager decided to hire someone more trustworthy, even if they were inexperienced...</t>
   </si>
   <si>
-    <t>23</t>
+    <t>27</t>
   </si>
   <si>
     <t>And then there were the customers.</t>
   </si>
   <si>
-    <t>25</t>
+    <t>29</t>
   </si>
   <si>
     <t>Touya</t>
@@ -128,13 +140,13 @@
     <t>"Welcome!"</t>
   </si>
   <si>
-    <t>27</t>
+    <t>31</t>
   </si>
   <si>
     <t>At this time it would usually be regular customers (unusual).</t>
   </si>
   <si>
-    <t>29</t>
+    <t>33</t>
   </si>
   <si>
     <t>Akira</t>
@@ -143,7 +155,7 @@
     <t>"Oh, Touya."</t>
   </si>
   <si>
-    <t>31</t>
+    <t>35</t>
   </si>
   <si>
     <t>Oh, it's Akira.</t>
@@ -152,25 +164,25 @@
     <t>What, it's Akira.</t>
   </si>
   <si>
-    <t>33</t>
+    <t>37</t>
   </si>
   <si>
     <t>"Touya, you're really taking this seriously, huh?"</t>
   </si>
   <si>
-    <t>35</t>
+    <t>39</t>
   </si>
   <si>
     <t>"Of course. You here for work today? Got customers?"</t>
   </si>
   <si>
-    <t>37</t>
+    <t>41</t>
   </si>
   <si>
     <t>"Hmmm? I was thinking of lending a hand."</t>
   </si>
   <si>
-    <t>39</t>
+    <t>43</t>
   </si>
   <si>
     <t>But since you're here, Touya, it's all good.</t>
@@ -179,7 +191,7 @@
     <t>"but with Touya here, it's all good."</t>
   </si>
   <si>
-    <t>41</t>
+    <t>45</t>
   </si>
   <si>
     <t>Eh, it's so-so.</t>
@@ -191,43 +203,43 @@
     <t>This phrase "いい加減だなあ…" is a colloquial expression in Japanese. It is often translated to English as "It's just so-so..." or "It's pretty mediocre..." It is an expression of disappointment or dissatisfaction with something that is not very good or not very bad. It can also be used to express dissatisfaction with someone's behavior or performance, meaning "It's pretty sloppy/careless."</t>
   </si>
   <si>
-    <t>43</t>
+    <t>47</t>
   </si>
   <si>
     <t>After all, it's Yuki and Shou who vouched for me to the shop manager here.</t>
   </si>
   <si>
-    <t>45</t>
+    <t>49</t>
   </si>
   <si>
     <t>To put it simply, the store manager is Shou's uncle.</t>
   </si>
   <si>
-    <t>47</t>
+    <t>51</t>
   </si>
   <si>
     <t>We were supposed to do this part-time job in shifts every day, since it was so tough.</t>
   </si>
   <si>
-    <t>49</t>
+    <t>53</t>
   </si>
   <si>
     <t>But eventually, it kind of turned into a mess.</t>
   </si>
   <si>
-    <t>51</t>
+    <t>55</t>
   </si>
   <si>
     <t>...Like Shou is now.</t>
   </si>
   <si>
-    <t>53</t>
+    <t>57</t>
   </si>
   <si>
     <t>Well, Shou has more of a compulsion to help out family members, so it might be fine for him.</t>
   </si>
   <si>
-    <t>55</t>
+    <t>59</t>
   </si>
   <si>
     <t>But I won't do it that way.</t>
@@ -237,43 +249,43 @@
 It translate to "But I can't do it that way." or "But I won't do it like that." It express a sense of refusal or disapproval with a situation or suggestion, or that the speaker has different plans or ideas.</t>
   </si>
   <si>
-    <t>57</t>
+    <t>61</t>
   </si>
   <si>
     <t>I am deeply grateful that the store manager lets me work freely, so I have been working here all this time.</t>
   </si>
   <si>
-    <t>59</t>
+    <t>63</t>
   </si>
   <si>
     <t>It's hard not to feel discouraged when I am slacking off.</t>
   </si>
   <si>
-    <t>61</t>
+    <t>65</t>
   </si>
   <si>
     <t>Touya?</t>
   </si>
   <si>
-    <t>63</t>
+    <t>67</t>
   </si>
   <si>
     <t>Huh?</t>
   </si>
   <si>
-    <t>65</t>
+    <t>69</t>
   </si>
   <si>
     <t>Can I order something?</t>
   </si>
   <si>
-    <t>67</t>
+    <t>71</t>
   </si>
   <si>
     <t>Yeah...</t>
   </si>
   <si>
-    <t>69</t>
+    <t>73</t>
   </si>
   <si>
     <t>What will you have?</t>
@@ -285,7 +297,7 @@
     <t>Weird inner monologue where he questions Touya's request to order, since Touya works there too.</t>
   </si>
   <si>
-    <t>71</t>
+    <t>75</t>
   </si>
   <si>
     <t>After all, you're a customer today.</t>
@@ -297,25 +309,25 @@
     <t>Ends with か but reads better as a statement.</t>
   </si>
   <si>
-    <t>73</t>
+    <t>77</t>
   </si>
   <si>
     <t>Then, Akira took his time to relax with a hot chocolate with cinnamon or something and then left by himself because he had a report to do.</t>
   </si>
   <si>
-    <t>75</t>
+    <t>79</t>
   </si>
   <si>
     <t>Looking at the clock, it's about time for the place to start getting crowded.</t>
   </si>
   <si>
-    <t>77</t>
+    <t>81</t>
   </si>
   <si>
     <t>Tonight, a few young people from the entertainment industry are occupying the cramped store.</t>
   </si>
   <si>
-    <t>79</t>
+    <t>83</t>
   </si>
   <si>
     <t>2</t>
@@ -330,13 +342,13 @@
     <t>"Touya-kun. I came to eat dinner."</t>
   </si>
   <si>
-    <t>81</t>
+    <t>85</t>
   </si>
   <si>
     <t>Oh, it's Yuki.</t>
   </si>
   <si>
-    <t>83</t>
+    <t>87</t>
   </si>
   <si>
     <t>0</t>
@@ -345,7 +357,7 @@
     <t>…………</t>
   </si>
   <si>
-    <t>85</t>
+    <t>89</t>
   </si>
   <si>
     <t>The expressionless girl I often see with Yuki is here, maybe she's a friend...?</t>
@@ -357,13 +369,13 @@
     <t>BEST GIRL</t>
   </si>
   <si>
-    <t>87</t>
+    <t>91</t>
   </si>
   <si>
     <t>Good work. What would you like?</t>
   </si>
   <si>
-    <t>89</t>
+    <t>93</t>
   </si>
   <si>
     <t>I ask the two girls sitting there while pouring water into a glass.</t>
@@ -372,19 +384,19 @@
     <t>I pour water into a glass while sitting at the counter, and ask the two people.</t>
   </si>
   <si>
-    <t>91</t>
+    <t>95</t>
   </si>
   <si>
     <t>No... I'm not finished yet. I have to go back to the studio again.</t>
   </si>
   <si>
-    <t>93</t>
+    <t>97</t>
   </si>
   <si>
     <t>"Really? That's tough, that means..."</t>
   </si>
   <si>
-    <t>95</t>
+    <t>99</t>
   </si>
   <si>
     <t>In reality, Yuki hasn't actually seen the Golden program she's in that's currently playing on the TV.</t>
@@ -393,13 +405,13 @@
     <t>In reality, Yuki hasn't actually watched the Golden program that she's on in real-time.</t>
   </si>
   <si>
-    <t>97</t>
+    <t>101</t>
   </si>
   <si>
     <t>Yuki: "It's not a big deal, it's not like I do it every day. Today is not for filming."</t>
   </si>
   <si>
-    <t>99</t>
+    <t>103</t>
   </si>
   <si>
     <t>Is that so?</t>
@@ -408,31 +420,31 @@
     <t>"I wonder if that's true...?"</t>
   </si>
   <si>
-    <t>101</t>
+    <t>105</t>
   </si>
   <si>
     <t>Even as I say that, I try not to interfere too much and listened to their orders.</t>
   </si>
   <si>
-    <t>103</t>
+    <t>107</t>
   </si>
   <si>
     <t>Tonight, there were some girls who seem to be new singers close to their debut (Yuki is a new singer too), and they were talking to Yuki in a way like "Senpai~", taking her away with them.</t>
   </si>
   <si>
-    <t>105</t>
+    <t>109</t>
   </si>
   <si>
     <t>"She's popular everywhere, huh..."</t>
   </si>
   <si>
-    <t>107</t>
+    <t>111</t>
   </si>
   <si>
     <t>I mutter to my lonely self.</t>
   </si>
   <si>
-    <t>109</t>
+    <t>113</t>
   </si>
   <si>
     <t>Yuki is teaching her juniors things like "the basics of gargling" in a way that sounds like an elder.</t>
@@ -444,7 +456,7 @@
     <t>This sentence is saying that Yuki on the TV program is teaching her junior colleagues things in a way that seems like she is older and more experienced. The sentence also specifically mentioned that she is teaching them something that is hard to understand, saying "she is teaching them things like 'the basic is gargling'(基本はうがいから)".</t>
   </si>
   <si>
-    <t>111</t>
+    <t>115</t>
   </si>
   <si>
     <t>6</t>
@@ -456,7 +468,7 @@
     <t>Um...</t>
   </si>
   <si>
-    <t>113</t>
+    <t>117</t>
   </si>
   <si>
     <t>Huh? Me?</t>
@@ -465,19 +477,19 @@
     <t>Yes? Is that me?</t>
   </si>
   <si>
-    <t>115</t>
+    <t>119</t>
   </si>
   <si>
     <t>That's the woman who's usually with Yuki.</t>
   </si>
   <si>
-    <t>117</t>
+    <t>121</t>
   </si>
   <si>
     <t>I'm sorry to disturb you, but is this your shop?</t>
   </si>
   <si>
-    <t>119</t>
+    <t>123</t>
   </si>
   <si>
     <t>No need to be so apologetic all of a sudden.</t>
@@ -486,7 +498,7 @@
     <t>No need to be so scared all of a sudden.</t>
   </si>
   <si>
-    <t>121</t>
+    <t>125</t>
   </si>
   <si>
     <t>Ah. Well, I work here part-time, but...?</t>
@@ -495,25 +507,25 @@
     <t>"Ah, I have a part-time job, but...?"</t>
   </si>
   <si>
-    <t>123</t>
+    <t>127</t>
   </si>
   <si>
     <t>"Are you friends with Yuki-san?"</t>
   </si>
   <si>
-    <t>125</t>
+    <t>129</t>
   </si>
   <si>
     <t>Eh...</t>
   </si>
   <si>
-    <t>127</t>
+    <t>131</t>
   </si>
   <si>
     <t>Friend...</t>
   </si>
   <si>
-    <t>129</t>
+    <t>133</t>
   </si>
   <si>
     <t>I mean, I guess so...</t>
@@ -522,19 +534,19 @@
     <t>If I'm saying that, then I guess so...</t>
   </si>
   <si>
-    <t>131</t>
+    <t>135</t>
   </si>
   <si>
     <t>"Well, I guess you could say that..."</t>
   </si>
   <si>
-    <t>133</t>
+    <t>137</t>
   </si>
   <si>
     <t>I wonder if Yuki really doesn't talk about her private life at work...</t>
   </si>
   <si>
-    <t>135</t>
+    <t>139</t>
   </si>
   <si>
     <t>Oh, I see. Excuse me.</t>
@@ -543,37 +555,37 @@
     <t>"Oh, I see. Excuse me."</t>
   </si>
   <si>
-    <t>137</t>
+    <t>141</t>
   </si>
   <si>
     <t>After that, the woman fell silent.</t>
   </si>
   <si>
-    <t>139</t>
+    <t>143</t>
   </si>
   <si>
     <t>Who is this person...?</t>
   </si>
   <si>
-    <t>141</t>
+    <t>145</t>
   </si>
   <si>
     <t>I should ask Yuki about it next time.</t>
   </si>
   <si>
-    <t>143</t>
+    <t>147</t>
   </si>
   <si>
     <t>I always think that and then forget.</t>
   </si>
   <si>
-    <t>145</t>
+    <t>149</t>
   </si>
   <si>
     <t>Yuki doesn't really like talking to me about work stuff.</t>
   </si>
   <si>
-    <t>147</t>
+    <t>151</t>
   </si>
   <si>
     <t>The Yuki on TV is causing her juniors trouble, saying things like "It's best to do gargling with salt dissolved in lukewarm water"</t>
@@ -585,37 +597,37 @@
     <t>This is referring to Yuki on the TV program</t>
   </si>
   <si>
-    <t>149</t>
+    <t>153</t>
   </si>
   <si>
     <t>"Sorry, Touya-kun. I gotta go soon even though I came all this way..."</t>
   </si>
   <si>
-    <t>151</t>
+    <t>155</t>
   </si>
   <si>
     <t>She then starts to prepare to leave, looking embarrassed from across the counter.</t>
   </si>
   <si>
-    <t>153</t>
+    <t>157</t>
   </si>
   <si>
     <t>"It's alright. We'll be at the same workplace tomorrow, you and me."</t>
   </si>
   <si>
-    <t>155</t>
+    <t>159</t>
   </si>
   <si>
     <t>"What...?"</t>
   </si>
   <si>
-    <t>157</t>
+    <t>161</t>
   </si>
   <si>
     <t>"What? What are you talking about? I'm doing a part-time job at the TV station tomorrow, as an AD."</t>
   </si>
   <si>
-    <t>159</t>
+    <t>163</t>
   </si>
   <si>
     <t>"Oh, what is this? I was surprised for a moment thinking that I had to come here tomorrow. Ahaha!"</t>
@@ -624,7 +636,7 @@
     <t>"Oh, what is this? I was surprised for a moment that I had to come here tomorrow. Haha..."</t>
   </si>
   <si>
-    <t>161</t>
+    <t>165</t>
   </si>
   <si>
     <t>Don't think around me, Yuki...</t>
@@ -633,12 +645,6 @@
     <t>Don't think with me as the center, Yuki...</t>
   </si>
   <si>
-    <t>163</t>
-  </si>
-  <si>
-    <t>165</t>
-  </si>
-  <si>
     <t>167</t>
   </si>
   <si>
@@ -654,28 +660,34 @@
     <t>175</t>
   </si>
   <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
     <t>Then Yuki was pulled away by the other woman and left.</t>
   </si>
   <si>
-    <t>177</t>
+    <t>181</t>
   </si>
   <si>
     <t>What a hurry.</t>
   </si>
   <si>
-    <t>179</t>
+    <t>183</t>
   </si>
   <si>
     <t>Poor Yuki, being with that woman like a clock.</t>
   </si>
   <si>
-    <t>181</t>
+    <t>185</t>
   </si>
   <si>
     <t>The busy time passes and somehow the customers disappear.</t>
   </si>
   <si>
-    <t>183</t>
+    <t>187</t>
   </si>
   <si>
     <t>I begin wiping the empty table and...huh?</t>
@@ -684,7 +696,7 @@
     <t>Wiping the empty table,</t>
   </si>
   <si>
-    <t>185</t>
+    <t>189</t>
   </si>
   <si>
     <t>Is that...?</t>
@@ -693,7 +705,7 @@
     <t>What's that...?</t>
   </si>
   <si>
-    <t>187</t>
+    <t>191</t>
   </si>
   <si>
     <t>The person sitting at that table is...</t>
@@ -702,91 +714,91 @@
     <t>Is that Ogata and Rina-chan sitting at that table...?</t>
   </si>
   <si>
-    <t>189</t>
+    <t>193</t>
   </si>
   <si>
     <t>Rina...Ogata-chan...</t>
   </si>
   <si>
-    <t>191</t>
+    <t>195</t>
   </si>
   <si>
     <t>No way...</t>
   </si>
   <si>
-    <t>193</t>
+    <t>197</t>
   </si>
   <si>
     <t>Rina Ogata is currently a top idol who is sharing the popularity with Yuki Morikawa at Ogata Productions.</t>
   </si>
   <si>
-    <t>195</t>
+    <t>199</t>
   </si>
   <si>
     <t>She is supposed to be the same age as Yuki, but she is technically one year more experienced and, from a skill point of view, I feel she is far above Yuki.</t>
   </si>
   <si>
-    <t>197</t>
+    <t>201</t>
   </si>
   <si>
     <t>I don't really understand it, but somehow...</t>
   </si>
   <si>
-    <t>199</t>
+    <t>203</t>
   </si>
   <si>
     <t>Yuki is naturally too private and is not followed by the media, whereas her image is fairly solidified.</t>
   </si>
   <si>
-    <t>201</t>
+    <t>205</t>
   </si>
   <si>
     <t>Her private self is never shown in front of the media.</t>
   </si>
   <si>
-    <t>203</t>
+    <t>207</t>
   </si>
   <si>
     <t>He seems to visit this place often, but I don't really recognize him.</t>
   </si>
   <si>
-    <t>205</t>
+    <t>209</t>
   </si>
   <si>
     <t>I didn't realize it when I first came in, but now that I'm suddenly so close, it feels kind of strange.</t>
   </si>
   <si>
-    <t>207</t>
+    <t>211</t>
   </si>
   <si>
     <t>It's like I've become na extra in a drama or something.</t>
   </si>
   <si>
-    <t>209</t>
+    <t>213</t>
   </si>
   <si>
     <t>Like there's a camera rolling somewhere.</t>
   </si>
   <si>
-    <t>211</t>
+    <t>215</t>
   </si>
   <si>
     <t>And today I'm with an older man.</t>
   </si>
   <si>
-    <t>213</t>
+    <t>217</t>
   </si>
   <si>
     <t>Is he a friend...?</t>
   </si>
   <si>
-    <t>215</t>
+    <t>219</t>
   </si>
   <si>
     <t>He just seems like a dirty old man...</t>
   </si>
   <si>
-    <t>217</t>
+    <t>221</t>
   </si>
   <si>
     <t>I shouldn't be making these kinds of judgements.</t>
@@ -795,13 +807,13 @@
     <t>I shouldn't be making such inquiries.</t>
   </si>
   <si>
-    <t>219</t>
+    <t>223</t>
   </si>
   <si>
     <t>I'll get serious about my work.</t>
   </si>
   <si>
-    <t>221</t>
+    <t>225</t>
   </si>
   <si>
     <t>4</t>
@@ -813,25 +825,25 @@
     <t>"...So, how many times do you expect me to say it?"</t>
   </si>
   <si>
-    <t>223</t>
+    <t>227</t>
   </si>
   <si>
     <t>Huh...?</t>
   </si>
   <si>
-    <t>225</t>
+    <t>229</t>
   </si>
   <si>
     <t>Though she was composed, it was obviously her who spoke in a cold and biting tone.</t>
   </si>
   <si>
-    <t>227</t>
+    <t>231</t>
   </si>
   <si>
     <t>I had an image of her being a tough daughter from watching TV, and it looks like it was right on the mark.</t>
   </si>
   <si>
-    <t>229</t>
+    <t>233</t>
   </si>
   <si>
     <t>Male Voice</t>
@@ -840,43 +852,43 @@
     <t>"I've been answering the same thing over and over again..."</t>
   </si>
   <si>
-    <t>231</t>
+    <t>235</t>
   </si>
   <si>
     <t>The other man responds nonchalantly.</t>
   </si>
   <si>
-    <t>233</t>
+    <t>237</t>
   </si>
   <si>
     <t>Upon closer inspection, it looks like this old man is a regular customer at this shop.</t>
   </si>
   <si>
-    <t>235</t>
+    <t>239</t>
   </si>
   <si>
     <t>Could he be related to the entertainment industry...?</t>
   </si>
   <si>
-    <t>237</t>
+    <t>241</t>
   </si>
   <si>
     <t>But it doesn't look like it...</t>
   </si>
   <si>
-    <t>239</t>
+    <t>243</t>
   </si>
   <si>
     <t>You're not really answering, are you?</t>
   </si>
   <si>
-    <t>241</t>
+    <t>245</t>
   </si>
   <si>
     <t>She sneers.</t>
   </si>
   <si>
-    <t>243</t>
+    <t>247</t>
   </si>
   <si>
     <t>"I've been trying to get out of it since a long time ago...!"</t>
@@ -885,49 +897,49 @@
     <t>"I'm just trying to get out of it since a while ago...!"</t>
   </si>
   <si>
-    <t>245</t>
+    <t>249</t>
   </si>
   <si>
     <t>"Hey, hey, hey. What kind of way is that to talk...? Stop talking like you're talking to a stranger."</t>
   </si>
   <si>
-    <t>247</t>
+    <t>251</t>
   </si>
   <si>
     <t>The flustered-looking old man grabs her arm.</t>
   </si>
   <si>
-    <t>249</t>
+    <t>253</t>
   </si>
   <si>
     <t>"Like a stranger? Is that different?"</t>
   </si>
   <si>
-    <t>251</t>
+    <t>255</t>
   </si>
   <si>
     <t>"If I keep doing things like this, I'm definitely going to get criticized by the media..."</t>
   </si>
   <si>
-    <t>253</t>
+    <t>257</t>
   </si>
   <si>
     <t>Media...?</t>
   </si>
   <si>
-    <t>255</t>
+    <t>259</t>
   </si>
   <si>
     <t>Is something going on...?</t>
   </si>
   <si>
-    <t>257</t>
+    <t>261</t>
   </si>
   <si>
     <t>"Hey, hey... Rina, you're misunderstanding. Let's calm down and talk about it..."</t>
   </si>
   <si>
-    <t>259</t>
+    <t>263</t>
   </si>
   <si>
     <t>Wa-wait...! That hurts! Don't use so much strength!</t>
@@ -936,13 +948,13 @@
     <t>"Wh-what... Stop! That hurts! Don't use so much strength!"</t>
   </si>
   <si>
-    <t>261</t>
+    <t>265</t>
   </si>
   <si>
     <t>"Don't misunderstand me... I like you the most, Rina-chan..."</t>
   </si>
   <si>
-    <t>263</t>
+    <t>267</t>
   </si>
   <si>
     <t>Wh-what's with "-chan"? It's disgusting! Don't call me Rina-chan!</t>
@@ -951,28 +963,28 @@
     <t>"Wh-what do you mean by 'I'?! That's disgusting!"</t>
   </si>
   <si>
-    <t>265</t>
+    <t>269</t>
   </si>
   <si>
     <t>Looks like they're in a perfect deadlock...</t>
   </si>
   <si>
-    <t>267</t>
+    <t>271</t>
   </si>
   <si>
     <t>Maybe I should intervene.</t>
   </si>
   <si>
-    <t>269</t>
-  </si>
-  <si>
-    <t>271</t>
+    <t>273</t>
+  </si>
+  <si>
+    <t>275</t>
   </si>
   <si>
     <t>As I draw closer to them, the man says,</t>
   </si>
   <si>
-    <t>273</t>
+    <t>277</t>
   </si>
   <si>
     <t>"Ah, dangerous..."</t>
@@ -981,19 +993,19 @@
     <t>Eiji is warning Touya that Rina's about to punch him.</t>
   </si>
   <si>
-    <t>275</t>
+    <t>279</t>
   </si>
   <si>
     <t>Suddenly, the man grabs my head and pulled me in.</t>
   </si>
   <si>
-    <t>277</t>
+    <t>281</t>
   </si>
   <si>
     <t>Eh...?</t>
   </si>
   <si>
-    <t>279</t>
+    <t>283</t>
   </si>
   <si>
     <t>A fist with tremendous force flies into my vision.</t>
@@ -1002,13 +1014,13 @@
     <t>A tremendous fist flies into my vision.</t>
   </si>
   <si>
-    <t>281</t>
+    <t>285</t>
   </si>
   <si>
     <t>I suddenly feel faint.</t>
   </si>
   <si>
-    <t>283</t>
+    <t>287</t>
   </si>
   <si>
     <t>Uwaa... I caught something. And... It's a rock. Terribly unlucky.</t>
@@ -1021,25 +1033,25 @@
 It translates to "Wow... It's in. And it's rock. You are so unlucky." It expresses a sense of surprise or disbelief when something unexpected happened, which is not in favor of the person spoken to, and might indicate the speaker finding it unfair, unfortunate or unlucky for the person spoken to. It also used an informal language and might be considered rude by some.</t>
   </si>
   <si>
-    <t>285</t>
+    <t>289</t>
   </si>
   <si>
     <t>"I don't know! It's your fault!"</t>
   </si>
   <si>
-    <t>287</t>
+    <t>291</t>
   </si>
   <si>
     <t>She shouted softly and then got up from her seat and left the store.</t>
   </si>
   <si>
-    <t>289</t>
+    <t>293</t>
   </si>
   <si>
     <t>...Are you alright, sir?</t>
   </si>
   <si>
-    <t>291</t>
+    <t>295</t>
   </si>
   <si>
     <t>N-no...</t>
@@ -1051,13 +1063,13 @@
     <t>The line is literally いいえ</t>
   </si>
   <si>
-    <t>293</t>
+    <t>297</t>
   </si>
   <si>
     <t>He's got such a cool face, shielding people like this... who is he?</t>
   </si>
   <si>
-    <t>295</t>
+    <t>299</t>
   </si>
   <si>
     <t>Here.</t>
@@ -1066,49 +1078,49 @@
     <t>Yes.</t>
   </si>
   <si>
-    <t>297</t>
+    <t>301</t>
   </si>
   <si>
     <t>He hands me several paper napkins.</t>
   </si>
   <si>
-    <t>299</t>
+    <t>303</t>
   </si>
   <si>
     <t>?</t>
   </si>
   <si>
-    <t>301</t>
+    <t>305</t>
   </si>
   <si>
     <t>Nosebleed.</t>
   </si>
   <si>
-    <t>303</t>
+    <t>307</t>
   </si>
   <si>
     <t>Ah...</t>
   </si>
   <si>
-    <t>305</t>
+    <t>309</t>
   </si>
   <si>
     <t>Hearing that, I place my hand near my nose.</t>
   </si>
   <si>
-    <t>307</t>
+    <t>311</t>
   </si>
   <si>
     <t>Ahh...</t>
   </si>
   <si>
-    <t>309</t>
+    <t>313</t>
   </si>
   <si>
     <t>It's bleeding.</t>
   </si>
   <si>
-    <t>311</t>
+    <t>315</t>
   </si>
   <si>
     <t>Sorry, man... I didn't think she'd actually hit you...</t>
@@ -1117,64 +1129,64 @@
     <t>君 makes it informal/friendly</t>
   </si>
   <si>
-    <t>313</t>
+    <t>317</t>
   </si>
   <si>
     <t>…………………</t>
   </si>
   <si>
-    <t>315</t>
+    <t>319</t>
   </si>
   <si>
     <t>While I lightly wipe my face with a handkerchief, I glare at the man with a frustrated look.</t>
   </si>
   <si>
-    <t>317</t>
+    <t>321</t>
   </si>
   <si>
     <t>"Uh, you don't look too happy. Alright, alright, I'll head home today."</t>
   </si>
   <si>
-    <t>319</t>
+    <t>323</t>
   </si>
   <si>
     <t>"I should take care of Rina's mood too."</t>
   </si>
   <si>
-    <t>321</t>
+    <t>325</t>
   </si>
   <si>
     <t>He gives a faint smile, as if he is troubled, and then walks towards the cashier.</t>
   </si>
   <si>
-    <t>323</t>
+    <t>327</t>
   </si>
   <si>
     <t>I, too, return to the back of the counter and wipe my face with a wet tissue once again.</t>
   </si>
   <si>
-    <t>325</t>
+    <t>329</t>
   </si>
   <si>
     <t>Just as he's about to leave,</t>
   </si>
   <si>
-    <t>327</t>
+    <t>331</t>
   </si>
   <si>
     <t>"I'm really sorry. I'll make sure to apologize properly next time."</t>
   </si>
   <si>
-    <t>329</t>
+    <t>333</t>
   </si>
   <si>
     <t>He peers out with a silly face.</t>
   </si>
   <si>
-    <t>331</t>
-  </si>
-  <si>
-    <t>333</t>
+    <t>335</t>
+  </si>
+  <si>
+    <t>337</t>
   </si>
   <si>
     <t>I look at the store manager while still sulking a bit.</t>
@@ -1183,7 +1195,7 @@
     <t>I still kind of feel sulky as I look at the store manager.</t>
   </si>
   <si>
-    <t>335</t>
+    <t>339</t>
   </si>
   <si>
     <t>He just looks at me as if to say "You're being overly dramatic."</t>
@@ -1192,7 +1204,7 @@
     <t>He just looks at me as if to say "Don't do anything extra".</t>
   </si>
   <si>
-    <t>337</t>
+    <t>341</t>
   </si>
   <si>
     <t>Well, maybe so...</t>
@@ -1201,7 +1213,7 @@
     <t>Well, maybe that's true...</t>
   </si>
   <si>
-    <t>339</t>
+    <t>343</t>
   </si>
   <si>
     <t>For the time being, I decide to leave early because I can't work anymore today.</t>
@@ -1627,10 +1639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J171"/>
+  <dimension ref="A1:J173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,19 +2077,19 @@
         <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>9</v>
@@ -2094,22 +2106,22 @@
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>9</v>
@@ -2126,22 +2138,22 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>9</v>
@@ -2158,22 +2170,22 @@
         <v>9</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>9</v>
@@ -2190,22 +2202,22 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>9</v>
@@ -2222,19 +2234,19 @@
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>48</v>
@@ -2260,7 +2272,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>9</v>
@@ -2289,19 +2301,19 @@
         <v>51</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>9</v>
@@ -2318,25 +2330,25 @@
         <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="H22" s="3" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>9</v>
@@ -2350,22 +2362,22 @@
         <v>9</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>9</v>
@@ -2382,25 +2394,25 @@
         <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>9</v>
@@ -2560,7 +2572,7 @@
         <v>71</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>9</v>
@@ -2574,22 +2586,22 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>9</v>
@@ -2606,25 +2618,25 @@
         <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>9</v>
@@ -2644,7 +2656,7 @@
         <v>9</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>9</v>
@@ -2673,10 +2685,10 @@
         <v>79</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>9</v>
@@ -2708,7 +2720,7 @@
         <v>9</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>9</v>
@@ -2740,7 +2752,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>9</v>
@@ -2772,19 +2784,19 @@
         <v>9</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="H36" s="3" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>9</v>
@@ -2798,25 +2810,25 @@
         <v>9</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>9</v>
@@ -2830,7 +2842,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>9</v>
@@ -2842,13 +2854,13 @@
         <v>9</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>9</v>
@@ -2862,25 +2874,25 @@
         <v>9</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="5" t="s">
+      <c r="H39" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>9</v>
@@ -2929,19 +2941,19 @@
         <v>99</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>9</v>
@@ -2958,7 +2970,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>9</v>
@@ -2973,7 +2985,7 @@
         <v>9</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>9</v>
@@ -2990,22 +3002,22 @@
         <v>9</v>
       </c>
       <c r="B43" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="4" t="s">
+      <c r="G43" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>9</v>
@@ -3022,25 +3034,25 @@
         <v>9</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="H44" s="3" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>9</v>
@@ -3054,22 +3066,22 @@
         <v>9</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>9</v>
+        <v>112</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>9</v>
@@ -3086,25 +3098,25 @@
         <v>9</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="2" t="s">
+      <c r="H46" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="I46" s="3" t="s">
         <v>9</v>
@@ -3118,22 +3130,22 @@
         <v>9</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>9</v>
@@ -3150,19 +3162,19 @@
         <v>9</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>121</v>
@@ -3185,19 +3197,19 @@
         <v>122</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>9</v>
@@ -3214,22 +3226,22 @@
         <v>9</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>9</v>
@@ -3246,22 +3258,22 @@
         <v>9</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="4" t="s">
+      <c r="G51" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>9</v>
@@ -3278,22 +3290,22 @@
         <v>9</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>9</v>
@@ -3310,19 +3322,19 @@
         <v>9</v>
       </c>
       <c r="B53" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>133</v>
@@ -3345,10 +3357,10 @@
         <v>134</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>9</v>
@@ -3409,22 +3421,22 @@
         <v>138</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G56" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="H56" s="3" t="s">
-        <v>141</v>
+        <v>9</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>9</v>
@@ -3438,13 +3450,13 @@
         <v>9</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>9</v>
@@ -3453,7 +3465,7 @@
         <v>9</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>9</v>
@@ -3470,25 +3482,25 @@
         <v>9</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>9</v>
+        <v>145</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>9</v>
@@ -3502,22 +3514,22 @@
         <v>9</v>
       </c>
       <c r="B59" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>9</v>
@@ -3534,19 +3546,19 @@
         <v>9</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>152</v>
@@ -3578,10 +3590,10 @@
         <v>9</v>
       </c>
       <c r="F61" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>155</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>9</v>
@@ -3598,22 +3610,22 @@
         <v>9</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G62" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>9</v>
@@ -3630,22 +3642,22 @@
         <v>9</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G63" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>9</v>
@@ -3662,19 +3674,19 @@
         <v>9</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>9</v>
+        <v>161</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>162</v>
@@ -3697,10 +3709,10 @@
         <v>163</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>9</v>
+        <v>147</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>9</v>
@@ -3729,19 +3741,19 @@
         <v>165</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F66" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>9</v>
@@ -3758,22 +3770,22 @@
         <v>9</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>9</v>
@@ -3790,19 +3802,19 @@
         <v>9</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>171</v>
@@ -3825,19 +3837,19 @@
         <v>172</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>143</v>
+        <v>10</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F69" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G69" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>9</v>
@@ -3854,22 +3866,22 @@
         <v>9</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G70" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>9</v>
@@ -3886,19 +3898,19 @@
         <v>9</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>178</v>
@@ -4026,13 +4038,13 @@
         <v>9</v>
       </c>
       <c r="F75" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="G75" s="5" t="s">
-        <v>187</v>
-      </c>
       <c r="H75" s="5" t="s">
-        <v>188</v>
+        <v>9</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>9</v>
@@ -4046,13 +4058,13 @@
         <v>9</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>9</v>
@@ -4061,7 +4073,7 @@
         <v>9</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>9</v>
@@ -4078,25 +4090,25 @@
         <v>9</v>
       </c>
       <c r="B77" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="G77" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G77" s="5" t="s">
+      <c r="H77" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>9</v>
@@ -4113,10 +4125,10 @@
         <v>193</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>9</v>
@@ -4145,10 +4157,10 @@
         <v>195</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>9</v>
@@ -4180,7 +4192,7 @@
         <v>10</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>9</v>
@@ -4209,19 +4221,19 @@
         <v>199</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F81" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>201</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>9</v>
@@ -4238,22 +4250,22 @@
         <v>9</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G82" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>9</v>
@@ -4270,22 +4282,22 @@
         <v>9</v>
       </c>
       <c r="B83" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G83" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G83" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="H83" s="5" t="s">
         <v>9</v>
@@ -4305,19 +4317,19 @@
         <v>206</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>9</v>
+        <v>207</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>9</v>
+        <v>208</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>9</v>
@@ -4334,13 +4346,13 @@
         <v>9</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>9</v>
@@ -4366,13 +4378,13 @@
         <v>9</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>143</v>
+        <v>10</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>9</v>
@@ -4398,13 +4410,13 @@
         <v>9</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>9</v>
@@ -4430,13 +4442,13 @@
         <v>9</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>9</v>
@@ -4462,13 +4474,13 @@
         <v>9</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>9</v>
@@ -4477,7 +4489,7 @@
         <v>9</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="H89" s="5" t="s">
         <v>9</v>
@@ -4494,13 +4506,13 @@
         <v>9</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>9</v>
@@ -4509,7 +4521,7 @@
         <v>9</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>9</v>
@@ -4602,10 +4614,10 @@
         <v>9</v>
       </c>
       <c r="F93" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G93" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="G93" s="5" t="s">
-        <v>221</v>
       </c>
       <c r="H93" s="5" t="s">
         <v>9</v>
@@ -4622,22 +4634,22 @@
         <v>9</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G94" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>224</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>9</v>
@@ -4654,22 +4666,22 @@
         <v>9</v>
       </c>
       <c r="B95" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="G95" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E95" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F95" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="G95" s="5" t="s">
-        <v>227</v>
       </c>
       <c r="H95" s="5" t="s">
         <v>9</v>
@@ -4686,22 +4698,22 @@
         <v>9</v>
       </c>
       <c r="B96" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G96" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>9</v>
@@ -4718,19 +4730,19 @@
         <v>9</v>
       </c>
       <c r="B97" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E97" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F97" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="G97" s="5" t="s">
         <v>231</v>
@@ -4762,10 +4774,10 @@
         <v>9</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>9</v>
+        <v>233</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>233</v>
+        <v>9</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>9</v>
@@ -5146,10 +5158,10 @@
         <v>9</v>
       </c>
       <c r="F110" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G110" s="3" t="s">
         <v>257</v>
-      </c>
-      <c r="G110" s="3" t="s">
-        <v>258</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>9</v>
@@ -5166,22 +5178,22 @@
         <v>9</v>
       </c>
       <c r="B111" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G111" s="5" t="s">
         <v>259</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E111" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F111" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G111" s="5" t="s">
-        <v>260</v>
       </c>
       <c r="H111" s="5" t="s">
         <v>9</v>
@@ -5198,22 +5210,22 @@
         <v>9</v>
       </c>
       <c r="B112" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F112" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="G112" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G112" s="3" t="s">
-        <v>264</v>
       </c>
       <c r="H112" s="3" t="s">
         <v>9</v>
@@ -5230,7 +5242,7 @@
         <v>9</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>9</v>
@@ -5245,7 +5257,7 @@
         <v>9</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H113" s="5" t="s">
         <v>9</v>
@@ -5262,13 +5274,13 @@
         <v>9</v>
       </c>
       <c r="B114" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D114" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>9</v>
@@ -5329,19 +5341,19 @@
         <v>271</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D116" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G116" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G116" s="3" t="s">
-        <v>273</v>
       </c>
       <c r="H116" s="3" t="s">
         <v>9</v>
@@ -5358,22 +5370,22 @@
         <v>9</v>
       </c>
       <c r="B117" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G117" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="C117" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D117" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F117" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G117" s="5" t="s">
-        <v>275</v>
       </c>
       <c r="H117" s="5" t="s">
         <v>9</v>
@@ -5390,13 +5402,13 @@
         <v>9</v>
       </c>
       <c r="B118" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D118" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>9</v>
@@ -5489,10 +5501,10 @@
         <v>282</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>262</v>
+        <v>9</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>263</v>
+        <v>9</v>
       </c>
       <c r="E121" s="4" t="s">
         <v>9</v>
@@ -5553,19 +5565,19 @@
         <v>286</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="E123" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F123" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G123" s="5" t="s">
         <v>287</v>
-      </c>
-      <c r="G123" s="5" t="s">
-        <v>288</v>
       </c>
       <c r="H123" s="5" t="s">
         <v>9</v>
@@ -5582,22 +5594,22 @@
         <v>9</v>
       </c>
       <c r="B124" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G124" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E124" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G124" s="3" t="s">
-        <v>290</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>9</v>
@@ -5614,19 +5626,19 @@
         <v>9</v>
       </c>
       <c r="B125" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F125" s="4" t="s">
         <v>291</v>
-      </c>
-      <c r="C125" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D125" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E125" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F125" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="G125" s="5" t="s">
         <v>292</v>
@@ -5649,10 +5661,10 @@
         <v>293</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>262</v>
+        <v>16</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>9</v>
@@ -5681,10 +5693,10 @@
         <v>295</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>262</v>
+        <v>9</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>263</v>
+        <v>9</v>
       </c>
       <c r="E127" s="4" t="s">
         <v>9</v>
@@ -5713,10 +5725,10 @@
         <v>297</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>9</v>
+        <v>266</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>9</v>
+        <v>267</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>9</v>
@@ -5745,10 +5757,10 @@
         <v>299</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>9</v>
+        <v>266</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>9</v>
+        <v>267</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>9</v>
@@ -5777,10 +5789,10 @@
         <v>301</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>272</v>
+        <v>9</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>9</v>
@@ -5809,19 +5821,19 @@
         <v>303</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>262</v>
+        <v>9</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>263</v>
+        <v>9</v>
       </c>
       <c r="E131" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F131" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G131" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="G131" s="5" t="s">
-        <v>305</v>
       </c>
       <c r="H131" s="5" t="s">
         <v>9</v>
@@ -5838,13 +5850,13 @@
         <v>9</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>9</v>
@@ -5853,7 +5865,7 @@
         <v>9</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H132" s="3" t="s">
         <v>9</v>
@@ -5870,22 +5882,22 @@
         <v>9</v>
       </c>
       <c r="B133" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F133" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="C133" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="D133" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="E133" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F133" s="4" t="s">
+      <c r="G133" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="G133" s="5" t="s">
-        <v>310</v>
       </c>
       <c r="H133" s="5" t="s">
         <v>9</v>
@@ -5902,22 +5914,22 @@
         <v>9</v>
       </c>
       <c r="B134" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G134" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G134" s="3" t="s">
-        <v>312</v>
       </c>
       <c r="H134" s="3" t="s">
         <v>9</v>
@@ -5934,19 +5946,19 @@
         <v>9</v>
       </c>
       <c r="B135" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F135" s="4" t="s">
         <v>313</v>
-      </c>
-      <c r="C135" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D135" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E135" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F135" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="G135" s="5" t="s">
         <v>314</v>
@@ -5969,10 +5981,10 @@
         <v>315</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>9</v>
@@ -5981,7 +5993,7 @@
         <v>9</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>145</v>
+        <v>316</v>
       </c>
       <c r="H136" s="3" t="s">
         <v>9</v>
@@ -5998,7 +6010,7 @@
         <v>9</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>9</v>
@@ -6013,7 +6025,7 @@
         <v>9</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H137" s="5" t="s">
         <v>9</v>
@@ -6030,13 +6042,13 @@
         <v>9</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>272</v>
+        <v>39</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>9</v>
@@ -6045,10 +6057,10 @@
         <v>9</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>319</v>
+        <v>149</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>320</v>
+        <v>9</v>
       </c>
       <c r="I138" s="3" t="s">
         <v>9</v>
@@ -6062,22 +6074,22 @@
         <v>9</v>
       </c>
       <c r="B139" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G139" s="5" t="s">
         <v>321</v>
-      </c>
-      <c r="C139" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D139" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E139" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F139" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G139" s="5" t="s">
-        <v>322</v>
       </c>
       <c r="H139" s="5" t="s">
         <v>9</v>
@@ -6094,25 +6106,25 @@
         <v>9</v>
       </c>
       <c r="B140" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G140" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C140" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E140" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G140" s="3" t="s">
+      <c r="H140" s="3" t="s">
         <v>324</v>
-      </c>
-      <c r="H140" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="I140" s="3" t="s">
         <v>9</v>
@@ -6138,10 +6150,10 @@
         <v>9</v>
       </c>
       <c r="F141" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G141" s="5" t="s">
         <v>326</v>
-      </c>
-      <c r="G141" s="5" t="s">
-        <v>327</v>
       </c>
       <c r="H141" s="5" t="s">
         <v>9</v>
@@ -6158,22 +6170,22 @@
         <v>9</v>
       </c>
       <c r="B142" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G142" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D142" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E142" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F142" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="G142" s="3" t="s">
-        <v>329</v>
       </c>
       <c r="H142" s="3" t="s">
         <v>9</v>
@@ -6190,25 +6202,25 @@
         <v>9</v>
       </c>
       <c r="B143" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E143" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F143" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="C143" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D143" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E143" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F143" s="4" t="s">
+      <c r="G143" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="G143" s="5" t="s">
-        <v>332</v>
-      </c>
       <c r="H143" s="5" t="s">
-        <v>333</v>
+        <v>9</v>
       </c>
       <c r="I143" s="5" t="s">
         <v>9</v>
@@ -6222,22 +6234,22 @@
         <v>9</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>262</v>
+        <v>9</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>263</v>
+        <v>9</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>9</v>
+        <v>333</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H144" s="3" t="s">
         <v>9</v>
@@ -6254,25 +6266,25 @@
         <v>9</v>
       </c>
       <c r="B145" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E145" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F145" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="G145" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="C145" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D145" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E145" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F145" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G145" s="5" t="s">
+      <c r="H145" s="5" t="s">
         <v>337</v>
-      </c>
-      <c r="H145" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="I145" s="5" t="s">
         <v>9</v>
@@ -6289,10 +6301,10 @@
         <v>338</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>16</v>
+        <v>266</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>9</v>
@@ -6321,22 +6333,22 @@
         <v>340</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E147" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F147" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G147" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="G147" s="5" t="s">
-        <v>342</v>
-      </c>
       <c r="H147" s="5" t="s">
-        <v>343</v>
+        <v>9</v>
       </c>
       <c r="I147" s="5" t="s">
         <v>9</v>
@@ -6350,13 +6362,13 @@
         <v>9</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>9</v>
+        <v>276</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>9</v>
@@ -6365,7 +6377,7 @@
         <v>9</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H148" s="3" t="s">
         <v>9</v>
@@ -6382,25 +6394,25 @@
         <v>9</v>
       </c>
       <c r="B149" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E149" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F149" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G149" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="C149" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D149" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E149" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F149" s="4" t="s">
+      <c r="H149" s="5" t="s">
         <v>347</v>
-      </c>
-      <c r="G149" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="H149" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="I149" s="5" t="s">
         <v>9</v>
@@ -6414,22 +6426,22 @@
         <v>9</v>
       </c>
       <c r="B150" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G150" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E150" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F150" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G150" s="3" t="s">
-        <v>350</v>
       </c>
       <c r="H150" s="3" t="s">
         <v>9</v>
@@ -6446,19 +6458,19 @@
         <v>9</v>
       </c>
       <c r="B151" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D151" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F151" s="4" t="s">
         <v>351</v>
-      </c>
-      <c r="C151" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D151" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E151" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F151" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="G151" s="5" t="s">
         <v>352</v>
@@ -6481,10 +6493,10 @@
         <v>353</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>272</v>
+        <v>9</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>9</v>
@@ -6516,7 +6528,7 @@
         <v>10</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E153" s="4" t="s">
         <v>9</v>
@@ -6545,10 +6557,10 @@
         <v>357</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>9</v>
+        <v>276</v>
       </c>
       <c r="E154" s="2" t="s">
         <v>9</v>
@@ -6577,10 +6589,10 @@
         <v>359</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E155" s="4" t="s">
         <v>9</v>
@@ -6641,10 +6653,10 @@
         <v>363</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>272</v>
+        <v>9</v>
       </c>
       <c r="E157" s="4" t="s">
         <v>9</v>
@@ -6656,7 +6668,7 @@
         <v>364</v>
       </c>
       <c r="H157" s="5" t="s">
-        <v>365</v>
+        <v>9</v>
       </c>
       <c r="I157" s="5" t="s">
         <v>9</v>
@@ -6670,22 +6682,22 @@
         <v>9</v>
       </c>
       <c r="B158" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G158" s="3" t="s">
         <v>366</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D158" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E158" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F158" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G158" s="3" t="s">
-        <v>367</v>
       </c>
       <c r="H158" s="3" t="s">
         <v>9</v>
@@ -6702,25 +6714,25 @@
         <v>9</v>
       </c>
       <c r="B159" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="C159" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F159" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G159" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="C159" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D159" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E159" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F159" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G159" s="5" t="s">
+      <c r="H159" s="5" t="s">
         <v>369</v>
-      </c>
-      <c r="H159" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="I159" s="5" t="s">
         <v>9</v>
@@ -6737,10 +6749,10 @@
         <v>370</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>272</v>
+        <v>39</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>9</v>
@@ -6769,10 +6781,10 @@
         <v>372</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>272</v>
+        <v>9</v>
       </c>
       <c r="E161" s="4" t="s">
         <v>9</v>
@@ -6801,10 +6813,10 @@
         <v>374</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>9</v>
+        <v>276</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>9</v>
@@ -6833,10 +6845,10 @@
         <v>376</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>9</v>
+        <v>276</v>
       </c>
       <c r="E163" s="4" t="s">
         <v>9</v>
@@ -6897,10 +6909,10 @@
         <v>380</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>272</v>
+        <v>9</v>
       </c>
       <c r="E165" s="4" t="s">
         <v>9</v>
@@ -6961,10 +6973,10 @@
         <v>384</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>35</v>
+        <v>276</v>
       </c>
       <c r="E167" s="4" t="s">
         <v>9</v>
@@ -6973,7 +6985,7 @@
         <v>9</v>
       </c>
       <c r="G167" s="5" t="s">
-        <v>367</v>
+        <v>385</v>
       </c>
       <c r="H167" s="5" t="s">
         <v>9</v>
@@ -6990,7 +7002,7 @@
         <v>9</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>9</v>
@@ -7002,7 +7014,7 @@
         <v>9</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>386</v>
+        <v>9</v>
       </c>
       <c r="G168" s="3" t="s">
         <v>387</v>
@@ -7025,19 +7037,19 @@
         <v>388</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E169" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F169" s="4" t="s">
-        <v>389</v>
+        <v>9</v>
       </c>
       <c r="G169" s="5" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="H169" s="5" t="s">
         <v>9</v>
@@ -7054,22 +7066,22 @@
         <v>9</v>
       </c>
       <c r="B170" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F170" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="G170" s="3" t="s">
         <v>391</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D170" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E170" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F170" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="G170" s="3" t="s">
-        <v>393</v>
       </c>
       <c r="H170" s="3" t="s">
         <v>9</v>
@@ -7086,30 +7098,94 @@
         <v>9</v>
       </c>
       <c r="B171" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="C171" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E171" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F171" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="G171" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="C171" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D171" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E171" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F171" s="4" t="s">
+      <c r="H171" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I171" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J171" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="G171" s="5" t="s">
+      <c r="C172" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F172" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="H171" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I171" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J171" s="5" t="s">
+      <c r="G172" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="H172" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I172" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J172" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A173" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E173" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F173" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G173" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="H173" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I173" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J173" s="5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add more missing lines
</commit_message>
<xml_diff>
--- a/tl/S00032.MES.BIN.xlsx
+++ b/tl/S00032.MES.BIN.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED3BBC8-8E66-46CE-8DDA-84BB6E7E506B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D47FD9-3D62-4488-88FA-88BDF903B277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4815" yWindow="11145" windowWidth="48240" windowHeight="19545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="410">
   <si>
     <t>Status</t>
   </si>
@@ -336,7 +336,7 @@
     <t>Yuki</t>
   </si>
   <si>
-    <t>"Touya-kun, I came to eat dinner."</t>
+    <t>"Touya-kun, I came here for dinner."</t>
   </si>
   <si>
     <t>"Touya-kun. I came to eat dinner."</t>
@@ -648,19 +648,46 @@
     <t>167</t>
   </si>
   <si>
+    <t>Yeah... So, it'd be great if we could meet tomorrow. But, I'll come here again too.</t>
+  </si>
+  <si>
     <t>169</t>
   </si>
   <si>
+    <t>Yeah. Come again. ...If you can, when I'm here.</t>
+  </si>
+  <si>
     <t>171</t>
   </si>
   <si>
+    <t>...Okay.</t>
+  </si>
+  <si>
+    <t>...Yeah.</t>
+  </si>
+  <si>
     <t>173</t>
   </si>
   <si>
+    <t>Let's hurry.</t>
+  </si>
+  <si>
     <t>175</t>
   </si>
   <si>
+    <t>O-okay...</t>
+  </si>
+  <si>
+    <t>Y-yeah...</t>
+  </si>
+  <si>
     <t>177</t>
+  </si>
+  <si>
+    <t>Well, see you...</t>
+  </si>
+  <si>
+    <t>Well then, bye...</t>
   </si>
   <si>
     <t>179</t>
@@ -1642,7 +1669,7 @@
   <dimension ref="A1:J173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4361,7 +4388,7 @@
         <v>9</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>9</v>
+        <v>210</v>
       </c>
       <c r="H85" s="5" t="s">
         <v>9</v>
@@ -4378,7 +4405,7 @@
         <v>9</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>10</v>
@@ -4393,7 +4420,7 @@
         <v>9</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>9</v>
+        <v>212</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>9</v>
@@ -4410,7 +4437,7 @@
         <v>9</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>104</v>
@@ -4422,10 +4449,10 @@
         <v>9</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>9</v>
+        <v>214</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>9</v>
+        <v>215</v>
       </c>
       <c r="H87" s="5" t="s">
         <v>9</v>
@@ -4442,7 +4469,7 @@
         <v>9</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>147</v>
@@ -4457,7 +4484,7 @@
         <v>9</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>9</v>
+        <v>217</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>9</v>
@@ -4474,7 +4501,7 @@
         <v>9</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>104</v>
@@ -4486,10 +4513,10 @@
         <v>9</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>9</v>
+        <v>219</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>9</v>
+        <v>220</v>
       </c>
       <c r="H89" s="5" t="s">
         <v>9</v>
@@ -4506,7 +4533,7 @@
         <v>9</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>104</v>
@@ -4518,10 +4545,10 @@
         <v>9</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>9</v>
+        <v>222</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>9</v>
+        <v>223</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>9</v>
@@ -4538,7 +4565,7 @@
         <v>9</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>9</v>
@@ -4553,7 +4580,7 @@
         <v>9</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="H91" s="5" t="s">
         <v>9</v>
@@ -4570,7 +4597,7 @@
         <v>9</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>9</v>
@@ -4585,7 +4612,7 @@
         <v>9</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>9</v>
@@ -4602,7 +4629,7 @@
         <v>9</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>9</v>
@@ -4617,7 +4644,7 @@
         <v>9</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="H93" s="5" t="s">
         <v>9</v>
@@ -4634,7 +4661,7 @@
         <v>9</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>9</v>
@@ -4649,7 +4676,7 @@
         <v>9</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>9</v>
@@ -4666,7 +4693,7 @@
         <v>9</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>9</v>
@@ -4678,10 +4705,10 @@
         <v>9</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="H95" s="5" t="s">
         <v>9</v>
@@ -4698,7 +4725,7 @@
         <v>9</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>9</v>
@@ -4710,10 +4737,10 @@
         <v>9</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>9</v>
@@ -4730,7 +4757,7 @@
         <v>9</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>9</v>
@@ -4742,10 +4769,10 @@
         <v>9</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="H97" s="5" t="s">
         <v>9</v>
@@ -4762,7 +4789,7 @@
         <v>9</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>9</v>
@@ -4774,7 +4801,7 @@
         <v>9</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>9</v>
@@ -4794,7 +4821,7 @@
         <v>9</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>9</v>
@@ -4809,7 +4836,7 @@
         <v>9</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="H99" s="5" t="s">
         <v>9</v>
@@ -4826,7 +4853,7 @@
         <v>9</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>9</v>
@@ -4841,7 +4868,7 @@
         <v>9</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="H100" s="3" t="s">
         <v>9</v>
@@ -4858,7 +4885,7 @@
         <v>9</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>9</v>
@@ -4873,7 +4900,7 @@
         <v>9</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>9</v>
@@ -4890,7 +4917,7 @@
         <v>9</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>9</v>
@@ -4905,7 +4932,7 @@
         <v>9</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>9</v>
@@ -4922,7 +4949,7 @@
         <v>9</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>9</v>
@@ -4937,7 +4964,7 @@
         <v>9</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="H103" s="5" t="s">
         <v>9</v>
@@ -4954,7 +4981,7 @@
         <v>9</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>9</v>
@@ -4969,7 +4996,7 @@
         <v>9</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>9</v>
@@ -4986,7 +5013,7 @@
         <v>9</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>9</v>
@@ -5001,7 +5028,7 @@
         <v>9</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="H105" s="5" t="s">
         <v>9</v>
@@ -5018,7 +5045,7 @@
         <v>9</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>9</v>
@@ -5033,7 +5060,7 @@
         <v>9</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>9</v>
@@ -5050,7 +5077,7 @@
         <v>9</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>9</v>
@@ -5065,7 +5092,7 @@
         <v>9</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="H107" s="5" t="s">
         <v>9</v>
@@ -5082,7 +5109,7 @@
         <v>9</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>9</v>
@@ -5097,7 +5124,7 @@
         <v>9</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>9</v>
@@ -5114,7 +5141,7 @@
         <v>9</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>9</v>
@@ -5129,7 +5156,7 @@
         <v>9</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="H109" s="5" t="s">
         <v>9</v>
@@ -5146,7 +5173,7 @@
         <v>9</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>9</v>
@@ -5161,7 +5188,7 @@
         <v>9</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>9</v>
@@ -5178,7 +5205,7 @@
         <v>9</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>9</v>
@@ -5193,7 +5220,7 @@
         <v>9</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="H111" s="5" t="s">
         <v>9</v>
@@ -5210,7 +5237,7 @@
         <v>9</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>9</v>
@@ -5222,10 +5249,10 @@
         <v>9</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="H112" s="3" t="s">
         <v>9</v>
@@ -5242,7 +5269,7 @@
         <v>9</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>9</v>
@@ -5257,7 +5284,7 @@
         <v>9</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="H113" s="5" t="s">
         <v>9</v>
@@ -5274,13 +5301,13 @@
         <v>9</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>9</v>
@@ -5289,7 +5316,7 @@
         <v>9</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>9</v>
@@ -5306,7 +5333,7 @@
         <v>9</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>9</v>
@@ -5321,7 +5348,7 @@
         <v>9</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="H115" s="5" t="s">
         <v>9</v>
@@ -5338,7 +5365,7 @@
         <v>9</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>9</v>
@@ -5353,7 +5380,7 @@
         <v>9</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="H116" s="3" t="s">
         <v>9</v>
@@ -5370,7 +5397,7 @@
         <v>9</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>9</v>
@@ -5385,7 +5412,7 @@
         <v>9</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="H117" s="5" t="s">
         <v>9</v>
@@ -5402,13 +5429,13 @@
         <v>9</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>9</v>
@@ -5417,7 +5444,7 @@
         <v>9</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="H118" s="3" t="s">
         <v>9</v>
@@ -5434,7 +5461,7 @@
         <v>9</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>9</v>
@@ -5449,7 +5476,7 @@
         <v>9</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="H119" s="5" t="s">
         <v>9</v>
@@ -5466,7 +5493,7 @@
         <v>9</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>9</v>
@@ -5481,7 +5508,7 @@
         <v>9</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="H120" s="3" t="s">
         <v>9</v>
@@ -5498,7 +5525,7 @@
         <v>9</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>9</v>
@@ -5513,7 +5540,7 @@
         <v>9</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="H121" s="5" t="s">
         <v>9</v>
@@ -5530,7 +5557,7 @@
         <v>9</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>9</v>
@@ -5545,7 +5572,7 @@
         <v>9</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="H122" s="3" t="s">
         <v>9</v>
@@ -5562,13 +5589,13 @@
         <v>9</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="E123" s="4" t="s">
         <v>9</v>
@@ -5577,7 +5604,7 @@
         <v>9</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="H123" s="5" t="s">
         <v>9</v>
@@ -5594,7 +5621,7 @@
         <v>9</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>9</v>
@@ -5609,7 +5636,7 @@
         <v>9</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>9</v>
@@ -5626,22 +5653,22 @@
         <v>9</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="E125" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="G125" s="5" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="H125" s="5" t="s">
         <v>9</v>
@@ -5658,13 +5685,13 @@
         <v>9</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>9</v>
@@ -5673,7 +5700,7 @@
         <v>9</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>9</v>
@@ -5690,7 +5717,7 @@
         <v>9</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>9</v>
@@ -5705,7 +5732,7 @@
         <v>9</v>
       </c>
       <c r="G127" s="5" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="H127" s="5" t="s">
         <v>9</v>
@@ -5722,13 +5749,13 @@
         <v>9</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>9</v>
@@ -5737,7 +5764,7 @@
         <v>9</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="H128" s="3" t="s">
         <v>9</v>
@@ -5754,13 +5781,13 @@
         <v>9</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>9</v>
@@ -5769,7 +5796,7 @@
         <v>9</v>
       </c>
       <c r="G129" s="5" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="H129" s="5" t="s">
         <v>9</v>
@@ -5786,7 +5813,7 @@
         <v>9</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>9</v>
@@ -5801,7 +5828,7 @@
         <v>9</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="H130" s="3" t="s">
         <v>9</v>
@@ -5818,7 +5845,7 @@
         <v>9</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>9</v>
@@ -5833,7 +5860,7 @@
         <v>9</v>
       </c>
       <c r="G131" s="5" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="H131" s="5" t="s">
         <v>9</v>
@@ -5850,13 +5877,13 @@
         <v>9</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>9</v>
@@ -5865,7 +5892,7 @@
         <v>9</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="H132" s="3" t="s">
         <v>9</v>
@@ -5882,22 +5909,22 @@
         <v>9</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="E133" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="G133" s="5" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="H133" s="5" t="s">
         <v>9</v>
@@ -5914,13 +5941,13 @@
         <v>9</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>9</v>
@@ -5929,7 +5956,7 @@
         <v>9</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="H134" s="3" t="s">
         <v>9</v>
@@ -5946,22 +5973,22 @@
         <v>9</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="E135" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F135" s="4" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="H135" s="5" t="s">
         <v>9</v>
@@ -5978,7 +6005,7 @@
         <v>9</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>9</v>
@@ -5993,7 +6020,7 @@
         <v>9</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="H136" s="3" t="s">
         <v>9</v>
@@ -6010,7 +6037,7 @@
         <v>9</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>9</v>
@@ -6025,7 +6052,7 @@
         <v>9</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="H137" s="5" t="s">
         <v>9</v>
@@ -6042,7 +6069,7 @@
         <v>9</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>10</v>
@@ -6074,7 +6101,7 @@
         <v>9</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>9</v>
@@ -6089,7 +6116,7 @@
         <v>9</v>
       </c>
       <c r="G139" s="5" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="H139" s="5" t="s">
         <v>9</v>
@@ -6106,13 +6133,13 @@
         <v>9</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>9</v>
@@ -6121,10 +6148,10 @@
         <v>9</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="I140" s="3" t="s">
         <v>9</v>
@@ -6138,7 +6165,7 @@
         <v>9</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>9</v>
@@ -6153,7 +6180,7 @@
         <v>9</v>
       </c>
       <c r="G141" s="5" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="H141" s="5" t="s">
         <v>9</v>
@@ -6170,7 +6197,7 @@
         <v>9</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>10</v>
@@ -6185,7 +6212,7 @@
         <v>9</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="H142" s="3" t="s">
         <v>9</v>
@@ -6202,7 +6229,7 @@
         <v>9</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>9</v>
@@ -6214,10 +6241,10 @@
         <v>9</v>
       </c>
       <c r="F143" s="4" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="G143" s="5" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="H143" s="5" t="s">
         <v>9</v>
@@ -6234,7 +6261,7 @@
         <v>9</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>9</v>
@@ -6246,10 +6273,10 @@
         <v>9</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="H144" s="3" t="s">
         <v>9</v>
@@ -6266,25 +6293,25 @@
         <v>9</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E145" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F145" s="4" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="G145" s="5" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="H145" s="5" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="I145" s="5" t="s">
         <v>9</v>
@@ -6298,13 +6325,13 @@
         <v>9</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>9</v>
@@ -6313,7 +6340,7 @@
         <v>9</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="H146" s="3" t="s">
         <v>9</v>
@@ -6330,7 +6357,7 @@
         <v>9</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>9</v>
@@ -6345,7 +6372,7 @@
         <v>9</v>
       </c>
       <c r="G147" s="5" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="H147" s="5" t="s">
         <v>9</v>
@@ -6362,13 +6389,13 @@
         <v>9</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>9</v>
@@ -6377,7 +6404,7 @@
         <v>9</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="H148" s="3" t="s">
         <v>9</v>
@@ -6394,7 +6421,7 @@
         <v>9</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>10</v>
@@ -6406,13 +6433,13 @@
         <v>9</v>
       </c>
       <c r="F149" s="4" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="G149" s="5" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="H149" s="5" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="I149" s="5" t="s">
         <v>9</v>
@@ -6426,7 +6453,7 @@
         <v>9</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>9</v>
@@ -6441,7 +6468,7 @@
         <v>9</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="H150" s="3" t="s">
         <v>9</v>
@@ -6458,22 +6485,22 @@
         <v>9</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E151" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="G151" s="5" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="H151" s="5" t="s">
         <v>9</v>
@@ -6490,7 +6517,7 @@
         <v>9</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>9</v>
@@ -6505,7 +6532,7 @@
         <v>9</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="H152" s="3" t="s">
         <v>9</v>
@@ -6522,7 +6549,7 @@
         <v>9</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>10</v>
@@ -6537,7 +6564,7 @@
         <v>9</v>
       </c>
       <c r="G153" s="5" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="H153" s="5" t="s">
         <v>9</v>
@@ -6554,13 +6581,13 @@
         <v>9</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E154" s="2" t="s">
         <v>9</v>
@@ -6569,7 +6596,7 @@
         <v>9</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="H154" s="3" t="s">
         <v>9</v>
@@ -6586,7 +6613,7 @@
         <v>9</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>10</v>
@@ -6601,7 +6628,7 @@
         <v>9</v>
       </c>
       <c r="G155" s="5" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="H155" s="5" t="s">
         <v>9</v>
@@ -6618,7 +6645,7 @@
         <v>9</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>9</v>
@@ -6633,7 +6660,7 @@
         <v>9</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="H156" s="3" t="s">
         <v>9</v>
@@ -6650,7 +6677,7 @@
         <v>9</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>9</v>
@@ -6665,7 +6692,7 @@
         <v>9</v>
       </c>
       <c r="G157" s="5" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="H157" s="5" t="s">
         <v>9</v>
@@ -6682,7 +6709,7 @@
         <v>9</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>9</v>
@@ -6697,7 +6724,7 @@
         <v>9</v>
       </c>
       <c r="G158" s="3" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="H158" s="3" t="s">
         <v>9</v>
@@ -6714,13 +6741,13 @@
         <v>9</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="C159" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E159" s="4" t="s">
         <v>9</v>
@@ -6729,10 +6756,10 @@
         <v>9</v>
       </c>
       <c r="G159" s="5" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="H159" s="5" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="I159" s="5" t="s">
         <v>9</v>
@@ -6746,7 +6773,7 @@
         <v>9</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>10</v>
@@ -6761,7 +6788,7 @@
         <v>9</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="H160" s="3" t="s">
         <v>9</v>
@@ -6778,7 +6805,7 @@
         <v>9</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="C161" s="4" t="s">
         <v>9</v>
@@ -6793,7 +6820,7 @@
         <v>9</v>
       </c>
       <c r="G161" s="5" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="H161" s="5" t="s">
         <v>9</v>
@@ -6810,13 +6837,13 @@
         <v>9</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>9</v>
@@ -6825,7 +6852,7 @@
         <v>9</v>
       </c>
       <c r="G162" s="3" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="H162" s="3" t="s">
         <v>9</v>
@@ -6842,13 +6869,13 @@
         <v>9</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E163" s="4" t="s">
         <v>9</v>
@@ -6857,7 +6884,7 @@
         <v>9</v>
       </c>
       <c r="G163" s="5" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="H163" s="5" t="s">
         <v>9</v>
@@ -6874,7 +6901,7 @@
         <v>9</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>9</v>
@@ -6889,7 +6916,7 @@
         <v>9</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="H164" s="3" t="s">
         <v>9</v>
@@ -6906,7 +6933,7 @@
         <v>9</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>9</v>
@@ -6921,7 +6948,7 @@
         <v>9</v>
       </c>
       <c r="G165" s="5" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="H165" s="5" t="s">
         <v>9</v>
@@ -6938,7 +6965,7 @@
         <v>9</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>9</v>
@@ -6953,7 +6980,7 @@
         <v>9</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="H166" s="3" t="s">
         <v>9</v>
@@ -6970,13 +6997,13 @@
         <v>9</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="C167" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E167" s="4" t="s">
         <v>9</v>
@@ -6985,7 +7012,7 @@
         <v>9</v>
       </c>
       <c r="G167" s="5" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="H167" s="5" t="s">
         <v>9</v>
@@ -7002,7 +7029,7 @@
         <v>9</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>9</v>
@@ -7017,7 +7044,7 @@
         <v>9</v>
       </c>
       <c r="G168" s="3" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="H168" s="3" t="s">
         <v>9</v>
@@ -7034,7 +7061,7 @@
         <v>9</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>10</v>
@@ -7049,7 +7076,7 @@
         <v>9</v>
       </c>
       <c r="G169" s="5" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="H169" s="5" t="s">
         <v>9</v>
@@ -7066,7 +7093,7 @@
         <v>9</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>9</v>
@@ -7078,10 +7105,10 @@
         <v>9</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="G170" s="3" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="H170" s="3" t="s">
         <v>9</v>
@@ -7098,7 +7125,7 @@
         <v>9</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="C171" s="4" t="s">
         <v>9</v>
@@ -7110,10 +7137,10 @@
         <v>9</v>
       </c>
       <c r="F171" s="4" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="G171" s="5" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="H171" s="5" t="s">
         <v>9</v>
@@ -7130,7 +7157,7 @@
         <v>9</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>9</v>
@@ -7142,10 +7169,10 @@
         <v>9</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="H172" s="3" t="s">
         <v>9</v>
@@ -7162,7 +7189,7 @@
         <v>9</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="C173" s="4" t="s">
         <v>9</v>
@@ -7174,10 +7201,10 @@
         <v>9</v>
       </c>
       <c r="F173" s="4" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="G173" s="5" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="H173" s="5" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Massive re-tl of S00032
</commit_message>
<xml_diff>
--- a/tl/S00032.MES.BIN.xlsx
+++ b/tl/S00032.MES.BIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B445FA89-D519-441C-99EC-B72BFB298600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFAB5B8-A8AD-44B6-A491-403A1ABBC8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="9810" windowWidth="45900" windowHeight="19845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="10500" windowWidth="45900" windowHeight="19845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00032.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="449">
   <si>
     <t>Status</t>
   </si>
@@ -50,18 +50,27 @@
     <t>1</t>
   </si>
   <si>
+    <t>I'm currently working my part-time job at "Echoes" this afternoon.</t>
+  </si>
+  <si>
     <t>Today I'm working at "Echoes" after lunch.</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
+    <t>I love this job because I can leave late, and most importantly, it's easy.</t>
+  </si>
+  <si>
     <t>I like this job because I can finish late and it's easy.</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
+    <t>Alright, time to work seriously.</t>
+  </si>
+  <si>
     <t>Alright, let's work seriously.</t>
   </si>
   <si>
@@ -80,24 +89,36 @@
     <t>11</t>
   </si>
   <si>
+    <t>Well, I can't say it's not due to that special environment, though.</t>
+  </si>
+  <si>
     <t>Well, I can't deny that it's because of that special environment.</t>
   </si>
   <si>
     <t>13</t>
   </si>
   <si>
+    <t>In other words, it creates an atmosphere that only regulars can enter.</t>
+  </si>
+  <si>
     <t>In other words, they've created an atmosphere where only regulars can get in.</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
+    <t>That created a problem when hiring part-timers.</t>
+  </si>
+  <si>
     <t>That was a problem when hiring part-timers.</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
+    <t>Mainly because the regulars are either from the entertainment industry, or aspiring entertainers taking lessons every day.</t>
+  </si>
+  <si>
     <t>Since the regulars are mostly related to the entertainment industry or aspiring entertainers who take lessons every day.</t>
   </si>
   <si>
@@ -110,12 +131,15 @@
     <t>21</t>
   </si>
   <si>
-    <t>They were going to hire a normal part-timer,</t>
+    <t>They were planning to hire a normal part-timer,</t>
   </si>
   <si>
     <t>23</t>
   </si>
   <si>
+    <t>but at the time of recruitment, it seemed like most of the people only showed up with the intention of meeting a celebrity.</t>
+  </si>
+  <si>
     <t>but at the time of recruitment, it seemed like a bunch of people who obviously came with the intention of meeting a celebrity had shown up.</t>
   </si>
   <si>
@@ -128,7 +152,7 @@
     <t>27</t>
   </si>
   <si>
-    <t>And then there were the customers.</t>
+    <t>Just now, a customer enters the shop.</t>
   </si>
   <si>
     <t>29</t>
@@ -143,6 +167,9 @@
     <t>31</t>
   </si>
   <si>
+    <t>This time, it's a normal customer (unusual).</t>
+  </si>
+  <si>
     <t>At this time it would usually be regular customers (unusual).</t>
   </si>
   <si>
@@ -152,13 +179,16 @@
     <t>Akira</t>
   </si>
   <si>
+    <t>Oh hey, Touya.</t>
+  </si>
+  <si>
     <t>"Oh, Touya."</t>
   </si>
   <si>
     <t>35</t>
   </si>
   <si>
-    <t>Oh, it's Akira.</t>
+    <t>Oh what, it's Akira.</t>
   </si>
   <si>
     <t>What, it's Akira.</t>
@@ -173,19 +203,22 @@
     <t>39</t>
   </si>
   <si>
+    <t>It's obvious, isn't it? Are you working today? Maybe dealing with customers?</t>
+  </si>
+  <si>
     <t>"Of course. You here for work today? Got customers?"</t>
   </si>
   <si>
     <t>41</t>
   </si>
   <si>
-    <t>"Hmmm? I was thinking of lending a hand."</t>
+    <t>"Hmmm? I was thinking of helping out."</t>
   </si>
   <si>
     <t>43</t>
   </si>
   <si>
-    <t>But since you're here, Touya, it's all good.</t>
+    <t>But everything looks to be fine with you here.</t>
   </si>
   <si>
     <t>"but with Touya here, it's all good."</t>
@@ -194,7 +227,7 @@
     <t>45</t>
   </si>
   <si>
-    <t>Eh, it's so-so.</t>
+    <t>That's a bit of a stretch...</t>
   </si>
   <si>
     <t>It's kinda rough, though...</t>
@@ -206,40 +239,61 @@
     <t>47</t>
   </si>
   <si>
+    <t>Yuki and Akira were the ones who originally vouched for me to the shop manager.</t>
+  </si>
+  <si>
     <t>After all, it's Yuki and Shou who vouched for me to the shop manager here.</t>
   </si>
   <si>
     <t>49</t>
   </si>
   <si>
+    <t>In short, the shop manager is Akira's uncle.</t>
+  </si>
+  <si>
     <t>To put it simply, the store manager is Shou's uncle.</t>
   </si>
   <si>
     <t>51</t>
   </si>
   <si>
+    <t>We were supposed to take turns doing this part-time job in shifts every day (since every day was too tough).</t>
+  </si>
+  <si>
     <t>We were supposed to do this part-time job in shifts every day, since it was so tough.</t>
   </si>
   <si>
     <t>53</t>
   </si>
   <si>
+    <t>But eventually, the rotation became kind of sloppy.</t>
+  </si>
+  <si>
     <t>But eventually, it kind of turned into a mess.</t>
   </si>
   <si>
     <t>55</t>
   </si>
   <si>
+    <t>...Like it is with Akira is now.</t>
+  </si>
+  <si>
     <t>...Like Shou is now.</t>
   </si>
   <si>
     <t>57</t>
   </si>
   <si>
+    <t>Well, I guess it's okay for him since he has family forcing him to help out.</t>
+  </si>
+  <si>
     <t>Well, Shou has more of a compulsion to help out family members, so it might be fine for him.</t>
   </si>
   <si>
     <t>59</t>
+  </si>
+  <si>
+    <t>But it's not okay for me.</t>
   </si>
   <si>
     <t>But I won't do it that way.</t>
@@ -252,12 +306,18 @@
     <t>61</t>
   </si>
   <si>
+    <t>I am deeply grateful that the store manager lets me work freely, so I've continued to work here all this time.</t>
+  </si>
+  <si>
     <t>I am deeply grateful that the store manager lets me work freely, so I have been working here all this time.</t>
   </si>
   <si>
     <t>63</t>
   </si>
   <si>
+    <t>I really can't stand someone who is carelessly lazy.</t>
+  </si>
+  <si>
     <t>It's hard not to feel discouraged when I am slacking off.</t>
   </si>
   <si>
@@ -282,13 +342,16 @@
     <t>71</t>
   </si>
   <si>
+    <t>Sure...</t>
+  </si>
+  <si>
     <t>Yeah...</t>
   </si>
   <si>
     <t>73</t>
   </si>
   <si>
-    <t>What will you have?</t>
+    <t>Tell me what it is.</t>
   </si>
   <si>
     <t>What is it?</t>
@@ -312,6 +375,9 @@
     <t>77</t>
   </si>
   <si>
+    <t>A bit later, after relaxing with a cinnamon-scented hot chocolate - or something - Akira leaves alone because he has a report to write.</t>
+  </si>
+  <si>
     <t>Then, Akira took his time to relax with a hot chocolate with cinnamon or something and then left by himself because he had a report to do.</t>
   </si>
   <si>
@@ -324,7 +390,7 @@
     <t>81</t>
   </si>
   <si>
-    <t>Tonight, a few young people from the entertainment industry are occupying the cramped store.</t>
+    <t>Tonight, a few young people from the entertainment industry are occupying the small shop.</t>
   </si>
   <si>
     <t>83</t>
@@ -360,7 +426,7 @@
     <t>89</t>
   </si>
   <si>
-    <t>The expressionless girl I often see with Yuki is here, maybe she's a friend...?</t>
+    <t>The expressionless woman I often see with Yuki is here, maybe she's a friend...?</t>
   </si>
   <si>
     <t>-I often see the expressionless girl who is with him, maybe she's a friend...?</t>
@@ -372,6 +438,9 @@
     <t>91</t>
   </si>
   <si>
+    <t>Good work today. What would you like?</t>
+  </si>
+  <si>
     <t>Good work. What would you like?</t>
   </si>
   <si>
@@ -408,7 +477,10 @@
     <t>101</t>
   </si>
   <si>
-    <t>Yuki: "It's not a big deal, it's not like I do it every day. Today is not for filming."</t>
+    <t>It's no different from usual. I'm not doing any filming today.</t>
+  </si>
+  <si>
+    <t>"It's not a big deal, it's not like I do it every day. Today is not for filming."</t>
   </si>
   <si>
     <t>103</t>
@@ -471,7 +543,7 @@
     <t>117</t>
   </si>
   <si>
-    <t>Huh? Me?</t>
+    <t>Yes? Are you talking to me?</t>
   </si>
   <si>
     <t>Yes? Is that me?</t>
@@ -486,7 +558,7 @@
     <t>121</t>
   </si>
   <si>
-    <t>I'm sorry to disturb you, but is this your shop?</t>
+    <t>I'm sorry to bother you, but is this your shop?</t>
   </si>
   <si>
     <t>123</t>
@@ -501,7 +573,7 @@
     <t>125</t>
   </si>
   <si>
-    <t>Ah. Well, I work here part-time, but...?</t>
+    <t>Ah. Well, I work here part-time, what about it...?</t>
   </si>
   <si>
     <t>"Ah, I have a part-time job, but...?"</t>
@@ -522,6 +594,9 @@
     <t>131</t>
   </si>
   <si>
+    <t>Friends...</t>
+  </si>
+  <si>
     <t>Friend...</t>
   </si>
   <si>
@@ -543,7 +618,7 @@
     <t>137</t>
   </si>
   <si>
-    <t>I wonder if Yuki really doesn't talk about her private life at work...</t>
+    <t>I wonder if Yuki really doesn't talk about her personal life at work...</t>
   </si>
   <si>
     <t>139</t>
@@ -558,24 +633,33 @@
     <t>141</t>
   </si>
   <si>
+    <t>After that, she falls silent.</t>
+  </si>
+  <si>
     <t>After that, the woman fell silent.</t>
   </si>
   <si>
     <t>143</t>
   </si>
   <si>
+    <t>Who is she...?</t>
+  </si>
+  <si>
     <t>Who is this person...?</t>
   </si>
   <si>
     <t>145</t>
   </si>
   <si>
-    <t>I should ask Yuki about it next time.</t>
+    <t>I should ask Yuki about her next time.</t>
   </si>
   <si>
     <t>147</t>
   </si>
   <si>
+    <t>I always think that and then forget to ask.</t>
+  </si>
+  <si>
     <t>I always think that and then forget.</t>
   </si>
   <si>
@@ -600,12 +684,18 @@
     <t>153</t>
   </si>
   <si>
+    <t>Sorry, Touya-kun. I have to leave now, even though I came all this way...</t>
+  </si>
+  <si>
     <t>"Sorry, Touya-kun. I gotta go soon even though I came all this way..."</t>
   </si>
   <si>
     <t>155</t>
   </si>
   <si>
+    <t>She then starts preparing to leave, looking embarrassed from across the counter.</t>
+  </si>
+  <si>
     <t>She then starts to prepare to leave, looking embarrassed from across the counter.</t>
   </si>
   <si>
@@ -618,19 +708,25 @@
     <t>159</t>
   </si>
   <si>
+    <t>...Huh?</t>
+  </si>
+  <si>
     <t>"What...?"</t>
   </si>
   <si>
     <t>161</t>
   </si>
   <si>
+    <t>Huh? What do you mean? I have a part-time job as an AD at the TV station tomorrow.</t>
+  </si>
+  <si>
     <t>"What? What are you talking about? I'm doing a part-time job at the TV station tomorrow, as an AD."</t>
   </si>
   <si>
     <t>163</t>
   </si>
   <si>
-    <t>"Oh, what is this? I was surprised for a moment thinking that I had to come here tomorrow. Ahaha!"</t>
+    <t>"Oh, no kidding. I was surprised for a moment thinking that I had to come here tomorrow. Ahaha!"</t>
   </si>
   <si>
     <t>"Oh, what is this? I was surprised for a moment that I had to come here tomorrow. Haha..."</t>
@@ -648,19 +744,25 @@
     <t>167</t>
   </si>
   <si>
+    <t>Alright. Well then, I hope to see you tomorrow. But I'll still come here again.</t>
+  </si>
+  <si>
     <t>Yeah... So, it'd be great if we could meet tomorrow. But, I'll come here again too.</t>
   </si>
   <si>
     <t>169</t>
   </si>
   <si>
+    <t>Yeah. Do come again. ...When I'm here, if you can help it.</t>
+  </si>
+  <si>
     <t>Yeah. Come again. ...If you can, when I'm here.</t>
   </si>
   <si>
     <t>171</t>
   </si>
   <si>
-    <t>...Okay.</t>
+    <t>...I will.</t>
   </si>
   <si>
     <t>...Yeah.</t>
@@ -669,6 +771,9 @@
     <t>173</t>
   </si>
   <si>
+    <t>Hurry up.</t>
+  </si>
+  <si>
     <t>Let's hurry.</t>
   </si>
   <si>
@@ -684,7 +789,7 @@
     <t>177</t>
   </si>
   <si>
-    <t>Well, see you...</t>
+    <t>See you later...</t>
   </si>
   <si>
     <t>Well then, bye...</t>
@@ -693,31 +798,43 @@
     <t>179</t>
   </si>
   <si>
+    <t>Yuki is then pulled away by the other woman and leaves.</t>
+  </si>
+  <si>
     <t>Then Yuki was pulled away by the other woman and left.</t>
   </si>
   <si>
     <t>181</t>
   </si>
   <si>
+    <t>Talk about hectic.</t>
+  </si>
+  <si>
     <t>What a hurry.</t>
   </si>
   <si>
     <t>183</t>
   </si>
   <si>
+    <t>Poor Yuki, being with that woman who operates like a clock.</t>
+  </si>
+  <si>
     <t>Poor Yuki, being with that woman like a clock.</t>
   </si>
   <si>
     <t>185</t>
   </si>
   <si>
+    <t>The busy time passes and some of the customers have left.</t>
+  </si>
+  <si>
     <t>The busy time passes and somehow the customers disappear.</t>
   </si>
   <si>
     <t>187</t>
   </si>
   <si>
-    <t>I begin wiping the empty table and...huh?</t>
+    <t>I begin wiping an empty table and...huh?</t>
   </si>
   <si>
     <t>Wiping the empty table,</t>
@@ -780,25 +897,25 @@
     <t>205</t>
   </si>
   <si>
-    <t>Her private self is never shown in front of the media.</t>
+    <t>Her private life is never shown in front of the media.</t>
   </si>
   <si>
     <t>207</t>
   </si>
   <si>
-    <t>He seems to visit this place often, but I don't really recognize him.</t>
+    <t>She seems to come to this shop often, but I haven't seen her much.</t>
   </si>
   <si>
     <t>209</t>
   </si>
   <si>
-    <t>I didn't realize it when I first came in, but now that I'm suddenly so close, it feels kind of strange.</t>
+    <t>I hadn't noticed her when I came in, but it feels strange to think she's suddenly here and so close.</t>
   </si>
   <si>
     <t>211</t>
   </si>
   <si>
-    <t>It's like I've become na extra in a drama or something.</t>
+    <t>It's like I've become an extra in a drama or something.</t>
   </si>
   <si>
     <t>213</t>
@@ -810,7 +927,7 @@
     <t>215</t>
   </si>
   <si>
-    <t>And today I'm with an older man.</t>
+    <t>Today she's with an older man.</t>
   </si>
   <si>
     <t>217</t>
@@ -1668,7 +1785,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1727,10 +1846,10 @@
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>9</v>
@@ -1747,7 +1866,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>9</v>
@@ -1759,10 +1878,10 @@
         <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>9</v>
@@ -1779,7 +1898,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
@@ -1791,10 +1910,10 @@
         <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>9</v>
@@ -1811,7 +1930,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>9</v>
@@ -1826,7 +1945,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>9</v>
@@ -1843,7 +1962,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
@@ -1858,7 +1977,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>9</v>
@@ -1875,7 +1994,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>9</v>
@@ -1887,10 +2006,10 @@
         <v>9</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>9</v>
@@ -1907,7 +2026,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
@@ -1919,10 +2038,10 @@
         <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>9</v>
@@ -1939,7 +2058,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -1951,10 +2070,10 @@
         <v>9</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>9</v>
@@ -1971,7 +2090,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>9</v>
@@ -1983,10 +2102,10 @@
         <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>9</v>
@@ -2003,7 +2122,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -2015,10 +2134,10 @@
         <v>9</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>9</v>
@@ -2035,7 +2154,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>9</v>
@@ -2050,7 +2169,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>9</v>
@@ -2067,7 +2186,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -2079,10 +2198,10 @@
         <v>9</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>9</v>
@@ -2099,7 +2218,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>9</v>
@@ -2114,7 +2233,7 @@
         <v>9</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>9</v>
@@ -2131,7 +2250,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -2146,7 +2265,7 @@
         <v>9</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>9</v>
@@ -2163,13 +2282,13 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>9</v>
@@ -2178,7 +2297,7 @@
         <v>9</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>9</v>
@@ -2195,7 +2314,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -2207,10 +2326,10 @@
         <v>9</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>9</v>
@@ -2227,22 +2346,22 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>9</v>
@@ -2259,7 +2378,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -2271,10 +2390,10 @@
         <v>9</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>9</v>
@@ -2291,13 +2410,13 @@
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>9</v>
@@ -2306,7 +2425,7 @@
         <v>9</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>9</v>
@@ -2323,22 +2442,22 @@
         <v>9</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>9</v>
@@ -2355,14 +2474,14 @@
         <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="E22" s="2" t="s">
         <v>9</v>
       </c>
@@ -2370,7 +2489,7 @@
         <v>9</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>9</v>
@@ -2387,22 +2506,22 @@
         <v>9</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>9</v>
@@ -2419,7 +2538,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>9</v>
@@ -2431,13 +2550,13 @@
         <v>9</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>9</v>
@@ -2451,7 +2570,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -2463,10 +2582,10 @@
         <v>9</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>9</v>
@@ -2483,7 +2602,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>9</v>
@@ -2495,10 +2614,10 @@
         <v>9</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>9</v>
@@ -2515,7 +2634,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -2527,10 +2646,10 @@
         <v>9</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>9</v>
@@ -2547,7 +2666,7 @@
         <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>9</v>
@@ -2559,10 +2678,10 @@
         <v>9</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>9</v>
@@ -2579,7 +2698,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -2591,10 +2710,10 @@
         <v>9</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>9</v>
@@ -2611,7 +2730,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>9</v>
@@ -2623,10 +2742,10 @@
         <v>9</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>9</v>
@@ -2643,7 +2762,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -2655,13 +2774,13 @@
         <v>9</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>9</v>
@@ -2675,7 +2794,7 @@
         <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>9</v>
@@ -2687,10 +2806,10 @@
         <v>9</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>9</v>
@@ -2707,7 +2826,7 @@
         <v>9</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -2719,10 +2838,10 @@
         <v>9</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>9</v>
@@ -2739,13 +2858,13 @@
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>9</v>
@@ -2754,7 +2873,7 @@
         <v>9</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>9</v>
@@ -2771,13 +2890,13 @@
         <v>9</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>9</v>
@@ -2786,7 +2905,7 @@
         <v>9</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>9</v>
@@ -2803,13 +2922,13 @@
         <v>9</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
@@ -2818,7 +2937,7 @@
         <v>9</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>9</v>
@@ -2835,22 +2954,22 @@
         <v>9</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>9</v>
@@ -2867,7 +2986,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>9</v>
@@ -2879,13 +2998,13 @@
         <v>9</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>9</v>
@@ -2899,7 +3018,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
@@ -2911,13 +3030,13 @@
         <v>9</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>9</v>
@@ -2931,7 +3050,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>9</v>
@@ -2943,10 +3062,10 @@
         <v>9</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>9</v>
@@ -2963,7 +3082,7 @@
         <v>9</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
@@ -2978,7 +3097,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>9</v>
@@ -2995,7 +3114,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>9</v>
@@ -3010,7 +3129,7 @@
         <v>9</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>9</v>
@@ -3027,22 +3146,22 @@
         <v>9</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>9</v>
@@ -3059,7 +3178,7 @@
         <v>9</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>9</v>
@@ -3074,7 +3193,7 @@
         <v>9</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>9</v>
@@ -3091,22 +3210,22 @@
         <v>9</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>9</v>
@@ -3123,7 +3242,7 @@
         <v>9</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>9</v>
@@ -3135,13 +3254,13 @@
         <v>9</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="I46" s="3" t="s">
         <v>9</v>
@@ -3155,22 +3274,22 @@
         <v>9</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>9</v>
+        <v>140</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>9</v>
@@ -3187,7 +3306,7 @@
         <v>9</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>9</v>
@@ -3199,10 +3318,10 @@
         <v>9</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>9</v>
@@ -3219,13 +3338,13 @@
         <v>9</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>9</v>
@@ -3234,7 +3353,7 @@
         <v>9</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>9</v>
@@ -3251,13 +3370,13 @@
         <v>9</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>9</v>
@@ -3266,7 +3385,7 @@
         <v>9</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>9</v>
@@ -3283,7 +3402,7 @@
         <v>9</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
@@ -3295,10 +3414,10 @@
         <v>9</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>9</v>
@@ -3315,22 +3434,22 @@
         <v>9</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>9</v>
+        <v>153</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>9</v>
@@ -3347,22 +3466,22 @@
         <v>9</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>9</v>
@@ -3379,7 +3498,7 @@
         <v>9</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>9</v>
@@ -3394,7 +3513,7 @@
         <v>9</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>9</v>
@@ -3411,7 +3530,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>9</v>
@@ -3426,7 +3545,7 @@
         <v>9</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>9</v>
@@ -3443,13 +3562,13 @@
         <v>9</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>9</v>
@@ -3458,7 +3577,7 @@
         <v>9</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>9</v>
@@ -3475,7 +3594,7 @@
         <v>9</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>9</v>
@@ -3490,7 +3609,7 @@
         <v>9</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>9</v>
@@ -3507,7 +3626,7 @@
         <v>9</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>9</v>
@@ -3519,13 +3638,13 @@
         <v>9</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>9</v>
@@ -3539,13 +3658,13 @@
         <v>9</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>9</v>
@@ -3554,7 +3673,7 @@
         <v>9</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>9</v>
@@ -3571,22 +3690,22 @@
         <v>9</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>9</v>
@@ -3603,7 +3722,7 @@
         <v>9</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>9</v>
@@ -3618,7 +3737,7 @@
         <v>9</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>9</v>
@@ -3635,13 +3754,13 @@
         <v>9</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>9</v>
@@ -3650,7 +3769,7 @@
         <v>9</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>9</v>
@@ -3667,7 +3786,7 @@
         <v>9</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>9</v>
@@ -3679,10 +3798,10 @@
         <v>9</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>9</v>
@@ -3699,22 +3818,22 @@
         <v>9</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>9</v>
@@ -3731,13 +3850,13 @@
         <v>9</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>9</v>
@@ -3746,7 +3865,7 @@
         <v>9</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="H65" s="5" t="s">
         <v>9</v>
@@ -3763,13 +3882,13 @@
         <v>9</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>9</v>
@@ -3778,7 +3897,7 @@
         <v>9</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>9</v>
@@ -3795,7 +3914,7 @@
         <v>9</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>9</v>
@@ -3807,10 +3926,10 @@
         <v>9</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>9</v>
+        <v>192</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>9</v>
@@ -3827,7 +3946,7 @@
         <v>9</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>9</v>
@@ -3839,10 +3958,10 @@
         <v>9</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>9</v>
@@ -3859,13 +3978,13 @@
         <v>9</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>172</v>
+        <v>197</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>9</v>
@@ -3874,7 +3993,7 @@
         <v>9</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>9</v>
@@ -3891,7 +4010,7 @@
         <v>9</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>9</v>
@@ -3906,7 +4025,7 @@
         <v>9</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>9</v>
@@ -3923,22 +4042,22 @@
         <v>9</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>9</v>
@@ -3955,7 +4074,7 @@
         <v>9</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>9</v>
@@ -3967,10 +4086,10 @@
         <v>9</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>9</v>
+        <v>205</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>9</v>
@@ -3987,7 +4106,7 @@
         <v>9</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>9</v>
@@ -3999,10 +4118,10 @@
         <v>9</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>9</v>
+        <v>208</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>9</v>
@@ -4019,7 +4138,7 @@
         <v>9</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>9</v>
@@ -4034,7 +4153,7 @@
         <v>9</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>184</v>
+        <v>211</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>9</v>
@@ -4051,7 +4170,7 @@
         <v>9</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>9</v>
@@ -4063,10 +4182,10 @@
         <v>9</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>9</v>
+        <v>213</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>186</v>
+        <v>214</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>9</v>
@@ -4083,7 +4202,7 @@
         <v>9</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>9</v>
@@ -4098,7 +4217,7 @@
         <v>9</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>9</v>
@@ -4115,7 +4234,7 @@
         <v>9</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>9</v>
@@ -4127,13 +4246,13 @@
         <v>9</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>190</v>
+        <v>218</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>192</v>
+        <v>220</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>9</v>
@@ -4147,22 +4266,22 @@
         <v>9</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>193</v>
+        <v>221</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>9</v>
+        <v>222</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>9</v>
@@ -4179,7 +4298,7 @@
         <v>9</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>195</v>
+        <v>224</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>9</v>
@@ -4191,10 +4310,10 @@
         <v>9</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>9</v>
+        <v>225</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
       <c r="H79" s="5" t="s">
         <v>9</v>
@@ -4211,13 +4330,13 @@
         <v>9</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>197</v>
+        <v>227</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>9</v>
@@ -4226,7 +4345,7 @@
         <v>9</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>198</v>
+        <v>228</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>9</v>
@@ -4243,22 +4362,22 @@
         <v>9</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>199</v>
+        <v>229</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>200</v>
+        <v>231</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>9</v>
@@ -4275,22 +4394,22 @@
         <v>9</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>201</v>
+        <v>232</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>9</v>
+        <v>233</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>9</v>
@@ -4307,22 +4426,22 @@
         <v>9</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>203</v>
+        <v>235</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>204</v>
+        <v>236</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>205</v>
+        <v>237</v>
       </c>
       <c r="H83" s="5" t="s">
         <v>9</v>
@@ -4339,7 +4458,7 @@
         <v>9</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>206</v>
+        <v>238</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>9</v>
@@ -4351,10 +4470,10 @@
         <v>9</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>207</v>
+        <v>239</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>208</v>
+        <v>240</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>9</v>
@@ -4371,22 +4490,22 @@
         <v>9</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>209</v>
+        <v>241</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>9</v>
+        <v>242</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>210</v>
+        <v>243</v>
       </c>
       <c r="H85" s="5" t="s">
         <v>9</v>
@@ -4403,22 +4522,22 @@
         <v>9</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>211</v>
+        <v>244</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>9</v>
+        <v>245</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>212</v>
+        <v>246</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>9</v>
@@ -4435,22 +4554,22 @@
         <v>9</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>214</v>
+        <v>248</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>215</v>
+        <v>249</v>
       </c>
       <c r="H87" s="5" t="s">
         <v>9</v>
@@ -4467,22 +4586,22 @@
         <v>9</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>216</v>
+        <v>250</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>9</v>
+        <v>251</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>217</v>
+        <v>252</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>9</v>
@@ -4499,22 +4618,22 @@
         <v>9</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>218</v>
+        <v>253</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>219</v>
+        <v>254</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="H89" s="5" t="s">
         <v>9</v>
@@ -4531,22 +4650,22 @@
         <v>9</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>221</v>
+        <v>256</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>222</v>
+        <v>257</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>223</v>
+        <v>258</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>9</v>
@@ -4563,7 +4682,7 @@
         <v>9</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>224</v>
+        <v>259</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>9</v>
@@ -4575,10 +4694,10 @@
         <v>9</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>9</v>
+        <v>260</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>225</v>
+        <v>261</v>
       </c>
       <c r="H91" s="5" t="s">
         <v>9</v>
@@ -4595,7 +4714,7 @@
         <v>9</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>226</v>
+        <v>262</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>9</v>
@@ -4607,10 +4726,10 @@
         <v>9</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>9</v>
+        <v>263</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>227</v>
+        <v>264</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>9</v>
@@ -4627,7 +4746,7 @@
         <v>9</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>228</v>
+        <v>265</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>9</v>
@@ -4639,10 +4758,10 @@
         <v>9</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>9</v>
+        <v>266</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>229</v>
+        <v>267</v>
       </c>
       <c r="H93" s="5" t="s">
         <v>9</v>
@@ -4659,7 +4778,7 @@
         <v>9</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>230</v>
+        <v>268</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>9</v>
@@ -4671,10 +4790,10 @@
         <v>9</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>9</v>
+        <v>269</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>231</v>
+        <v>270</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>9</v>
@@ -4691,7 +4810,7 @@
         <v>9</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>9</v>
@@ -4703,10 +4822,10 @@
         <v>9</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="H95" s="5" t="s">
         <v>9</v>
@@ -4723,7 +4842,7 @@
         <v>9</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>235</v>
+        <v>274</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>9</v>
@@ -4735,10 +4854,10 @@
         <v>9</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>236</v>
+        <v>275</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>237</v>
+        <v>276</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>9</v>
@@ -4755,7 +4874,7 @@
         <v>9</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>238</v>
+        <v>277</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>9</v>
@@ -4767,10 +4886,10 @@
         <v>9</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>239</v>
+        <v>278</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>240</v>
+        <v>279</v>
       </c>
       <c r="H97" s="5" t="s">
         <v>9</v>
@@ -4787,7 +4906,7 @@
         <v>9</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>241</v>
+        <v>280</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>9</v>
@@ -4799,7 +4918,7 @@
         <v>9</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>242</v>
+        <v>281</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>9</v>
@@ -4819,7 +4938,7 @@
         <v>9</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>243</v>
+        <v>282</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>9</v>
@@ -4834,7 +4953,7 @@
         <v>9</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>244</v>
+        <v>283</v>
       </c>
       <c r="H99" s="5" t="s">
         <v>9</v>
@@ -4851,7 +4970,7 @@
         <v>9</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>245</v>
+        <v>284</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>9</v>
@@ -4866,7 +4985,7 @@
         <v>9</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>246</v>
+        <v>285</v>
       </c>
       <c r="H100" s="3" t="s">
         <v>9</v>
@@ -4883,7 +5002,7 @@
         <v>9</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>247</v>
+        <v>286</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>9</v>
@@ -4898,7 +5017,7 @@
         <v>9</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>248</v>
+        <v>287</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>9</v>
@@ -4915,7 +5034,7 @@
         <v>9</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>249</v>
+        <v>288</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>9</v>
@@ -4930,7 +5049,7 @@
         <v>9</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>250</v>
+        <v>289</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>9</v>
@@ -4947,7 +5066,7 @@
         <v>9</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>251</v>
+        <v>290</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>9</v>
@@ -4962,7 +5081,7 @@
         <v>9</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>252</v>
+        <v>291</v>
       </c>
       <c r="H103" s="5" t="s">
         <v>9</v>
@@ -4979,7 +5098,7 @@
         <v>9</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>253</v>
+        <v>292</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>9</v>
@@ -4994,7 +5113,7 @@
         <v>9</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>254</v>
+        <v>293</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>9</v>
@@ -5011,7 +5130,7 @@
         <v>9</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>255</v>
+        <v>294</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>9</v>
@@ -5026,7 +5145,7 @@
         <v>9</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="H105" s="5" t="s">
         <v>9</v>
@@ -5043,7 +5162,7 @@
         <v>9</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>9</v>
@@ -5058,7 +5177,7 @@
         <v>9</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>258</v>
+        <v>297</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>9</v>
@@ -5075,7 +5194,7 @@
         <v>9</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>259</v>
+        <v>298</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>9</v>
@@ -5090,7 +5209,7 @@
         <v>9</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>260</v>
+        <v>299</v>
       </c>
       <c r="H107" s="5" t="s">
         <v>9</v>
@@ -5107,7 +5226,7 @@
         <v>9</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>261</v>
+        <v>300</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>9</v>
@@ -5122,7 +5241,7 @@
         <v>9</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>262</v>
+        <v>301</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>9</v>
@@ -5139,7 +5258,7 @@
         <v>9</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>263</v>
+        <v>302</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>9</v>
@@ -5154,7 +5273,7 @@
         <v>9</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>264</v>
+        <v>303</v>
       </c>
       <c r="H109" s="5" t="s">
         <v>9</v>
@@ -5171,7 +5290,7 @@
         <v>9</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>265</v>
+        <v>304</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>9</v>
@@ -5186,7 +5305,7 @@
         <v>9</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>266</v>
+        <v>305</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>9</v>
@@ -5203,7 +5322,7 @@
         <v>9</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>267</v>
+        <v>306</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>9</v>
@@ -5218,7 +5337,7 @@
         <v>9</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>268</v>
+        <v>307</v>
       </c>
       <c r="H111" s="5" t="s">
         <v>9</v>
@@ -5235,7 +5354,7 @@
         <v>9</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>269</v>
+        <v>308</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>9</v>
@@ -5247,10 +5366,10 @@
         <v>9</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>270</v>
+        <v>309</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>271</v>
+        <v>310</v>
       </c>
       <c r="H112" s="3" t="s">
         <v>9</v>
@@ -5267,7 +5386,7 @@
         <v>9</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>272</v>
+        <v>311</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>9</v>
@@ -5282,7 +5401,7 @@
         <v>9</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>273</v>
+        <v>312</v>
       </c>
       <c r="H113" s="5" t="s">
         <v>9</v>
@@ -5299,13 +5418,13 @@
         <v>9</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>274</v>
+        <v>313</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>276</v>
+        <v>315</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>9</v>
@@ -5314,7 +5433,7 @@
         <v>9</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>277</v>
+        <v>316</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>9</v>
@@ -5331,7 +5450,7 @@
         <v>9</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>278</v>
+        <v>317</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>9</v>
@@ -5346,7 +5465,7 @@
         <v>9</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>279</v>
+        <v>318</v>
       </c>
       <c r="H115" s="5" t="s">
         <v>9</v>
@@ -5363,7 +5482,7 @@
         <v>9</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>280</v>
+        <v>319</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>9</v>
@@ -5378,7 +5497,7 @@
         <v>9</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>281</v>
+        <v>320</v>
       </c>
       <c r="H116" s="3" t="s">
         <v>9</v>
@@ -5395,7 +5514,7 @@
         <v>9</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>282</v>
+        <v>321</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>9</v>
@@ -5410,7 +5529,7 @@
         <v>9</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>283</v>
+        <v>322</v>
       </c>
       <c r="H117" s="5" t="s">
         <v>9</v>
@@ -5427,13 +5546,13 @@
         <v>9</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>284</v>
+        <v>323</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>9</v>
@@ -5442,7 +5561,7 @@
         <v>9</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>286</v>
+        <v>325</v>
       </c>
       <c r="H118" s="3" t="s">
         <v>9</v>
@@ -5459,7 +5578,7 @@
         <v>9</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>287</v>
+        <v>326</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>9</v>
@@ -5474,7 +5593,7 @@
         <v>9</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>288</v>
+        <v>327</v>
       </c>
       <c r="H119" s="5" t="s">
         <v>9</v>
@@ -5491,7 +5610,7 @@
         <v>9</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>289</v>
+        <v>328</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>9</v>
@@ -5506,7 +5625,7 @@
         <v>9</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>290</v>
+        <v>329</v>
       </c>
       <c r="H120" s="3" t="s">
         <v>9</v>
@@ -5523,7 +5642,7 @@
         <v>9</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>291</v>
+        <v>330</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>9</v>
@@ -5538,7 +5657,7 @@
         <v>9</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>292</v>
+        <v>331</v>
       </c>
       <c r="H121" s="5" t="s">
         <v>9</v>
@@ -5555,7 +5674,7 @@
         <v>9</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>293</v>
+        <v>332</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>9</v>
@@ -5570,7 +5689,7 @@
         <v>9</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>294</v>
+        <v>333</v>
       </c>
       <c r="H122" s="3" t="s">
         <v>9</v>
@@ -5587,13 +5706,13 @@
         <v>9</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>295</v>
+        <v>334</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>276</v>
+        <v>315</v>
       </c>
       <c r="E123" s="4" t="s">
         <v>9</v>
@@ -5602,7 +5721,7 @@
         <v>9</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
       <c r="H123" s="5" t="s">
         <v>9</v>
@@ -5619,7 +5738,7 @@
         <v>9</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>297</v>
+        <v>336</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>9</v>
@@ -5634,7 +5753,7 @@
         <v>9</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>298</v>
+        <v>337</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>9</v>
@@ -5651,22 +5770,22 @@
         <v>9</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>299</v>
+        <v>338</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>276</v>
+        <v>315</v>
       </c>
       <c r="E125" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>300</v>
+        <v>339</v>
       </c>
       <c r="G125" s="5" t="s">
-        <v>301</v>
+        <v>340</v>
       </c>
       <c r="H125" s="5" t="s">
         <v>9</v>
@@ -5683,13 +5802,13 @@
         <v>9</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>302</v>
+        <v>341</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>9</v>
@@ -5698,7 +5817,7 @@
         <v>9</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>303</v>
+        <v>342</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>9</v>
@@ -5715,7 +5834,7 @@
         <v>9</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>304</v>
+        <v>343</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>9</v>
@@ -5730,7 +5849,7 @@
         <v>9</v>
       </c>
       <c r="G127" s="5" t="s">
-        <v>305</v>
+        <v>344</v>
       </c>
       <c r="H127" s="5" t="s">
         <v>9</v>
@@ -5747,13 +5866,13 @@
         <v>9</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>306</v>
+        <v>345</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>276</v>
+        <v>315</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>9</v>
@@ -5762,7 +5881,7 @@
         <v>9</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>307</v>
+        <v>346</v>
       </c>
       <c r="H128" s="3" t="s">
         <v>9</v>
@@ -5779,13 +5898,13 @@
         <v>9</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>308</v>
+        <v>347</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>276</v>
+        <v>315</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>9</v>
@@ -5794,7 +5913,7 @@
         <v>9</v>
       </c>
       <c r="G129" s="5" t="s">
-        <v>309</v>
+        <v>348</v>
       </c>
       <c r="H129" s="5" t="s">
         <v>9</v>
@@ -5811,7 +5930,7 @@
         <v>9</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>310</v>
+        <v>349</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>9</v>
@@ -5826,7 +5945,7 @@
         <v>9</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>311</v>
+        <v>350</v>
       </c>
       <c r="H130" s="3" t="s">
         <v>9</v>
@@ -5843,7 +5962,7 @@
         <v>9</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>312</v>
+        <v>351</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>9</v>
@@ -5858,7 +5977,7 @@
         <v>9</v>
       </c>
       <c r="G131" s="5" t="s">
-        <v>313</v>
+        <v>352</v>
       </c>
       <c r="H131" s="5" t="s">
         <v>9</v>
@@ -5875,13 +5994,13 @@
         <v>9</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>314</v>
+        <v>353</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>9</v>
@@ -5890,7 +6009,7 @@
         <v>9</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>315</v>
+        <v>354</v>
       </c>
       <c r="H132" s="3" t="s">
         <v>9</v>
@@ -5907,22 +6026,22 @@
         <v>9</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>316</v>
+        <v>355</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>276</v>
+        <v>315</v>
       </c>
       <c r="E133" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>317</v>
+        <v>356</v>
       </c>
       <c r="G133" s="5" t="s">
-        <v>318</v>
+        <v>357</v>
       </c>
       <c r="H133" s="5" t="s">
         <v>9</v>
@@ -5939,13 +6058,13 @@
         <v>9</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>319</v>
+        <v>358</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>9</v>
@@ -5954,7 +6073,7 @@
         <v>9</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>320</v>
+        <v>359</v>
       </c>
       <c r="H134" s="3" t="s">
         <v>9</v>
@@ -5971,22 +6090,22 @@
         <v>9</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>276</v>
+        <v>315</v>
       </c>
       <c r="E135" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F135" s="4" t="s">
-        <v>322</v>
+        <v>361</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>323</v>
+        <v>362</v>
       </c>
       <c r="H135" s="5" t="s">
         <v>9</v>
@@ -6003,7 +6122,7 @@
         <v>9</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>324</v>
+        <v>363</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>9</v>
@@ -6018,7 +6137,7 @@
         <v>9</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>325</v>
+        <v>364</v>
       </c>
       <c r="H136" s="3" t="s">
         <v>9</v>
@@ -6035,7 +6154,7 @@
         <v>9</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>326</v>
+        <v>365</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>9</v>
@@ -6050,7 +6169,7 @@
         <v>9</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>327</v>
+        <v>366</v>
       </c>
       <c r="H137" s="5" t="s">
         <v>9</v>
@@ -6067,13 +6186,13 @@
         <v>9</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>328</v>
+        <v>367</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>9</v>
@@ -6082,7 +6201,7 @@
         <v>9</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="H138" s="3" t="s">
         <v>9</v>
@@ -6099,7 +6218,7 @@
         <v>9</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>329</v>
+        <v>368</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>9</v>
@@ -6114,7 +6233,7 @@
         <v>9</v>
       </c>
       <c r="G139" s="5" t="s">
-        <v>330</v>
+        <v>369</v>
       </c>
       <c r="H139" s="5" t="s">
         <v>9</v>
@@ -6131,13 +6250,13 @@
         <v>9</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>331</v>
+        <v>370</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>9</v>
@@ -6146,10 +6265,10 @@
         <v>9</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>332</v>
+        <v>371</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>333</v>
+        <v>372</v>
       </c>
       <c r="I140" s="3" t="s">
         <v>9</v>
@@ -6163,7 +6282,7 @@
         <v>9</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>334</v>
+        <v>373</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>9</v>
@@ -6178,7 +6297,7 @@
         <v>9</v>
       </c>
       <c r="G141" s="5" t="s">
-        <v>335</v>
+        <v>374</v>
       </c>
       <c r="H141" s="5" t="s">
         <v>9</v>
@@ -6195,13 +6314,13 @@
         <v>9</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>336</v>
+        <v>375</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>9</v>
@@ -6210,7 +6329,7 @@
         <v>9</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>337</v>
+        <v>376</v>
       </c>
       <c r="H142" s="3" t="s">
         <v>9</v>
@@ -6227,7 +6346,7 @@
         <v>9</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>338</v>
+        <v>377</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>9</v>
@@ -6239,10 +6358,10 @@
         <v>9</v>
       </c>
       <c r="F143" s="4" t="s">
-        <v>339</v>
+        <v>378</v>
       </c>
       <c r="G143" s="5" t="s">
-        <v>340</v>
+        <v>379</v>
       </c>
       <c r="H143" s="5" t="s">
         <v>9</v>
@@ -6259,7 +6378,7 @@
         <v>9</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>341</v>
+        <v>380</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>9</v>
@@ -6271,10 +6390,10 @@
         <v>9</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>342</v>
+        <v>381</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>342</v>
+        <v>381</v>
       </c>
       <c r="H144" s="3" t="s">
         <v>9</v>
@@ -6291,25 +6410,25 @@
         <v>9</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>343</v>
+        <v>382</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E145" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F145" s="4" t="s">
-        <v>344</v>
+        <v>383</v>
       </c>
       <c r="G145" s="5" t="s">
-        <v>345</v>
+        <v>384</v>
       </c>
       <c r="H145" s="5" t="s">
-        <v>346</v>
+        <v>385</v>
       </c>
       <c r="I145" s="5" t="s">
         <v>9</v>
@@ -6323,13 +6442,13 @@
         <v>9</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>347</v>
+        <v>386</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>276</v>
+        <v>315</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>9</v>
@@ -6338,7 +6457,7 @@
         <v>9</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>348</v>
+        <v>387</v>
       </c>
       <c r="H146" s="3" t="s">
         <v>9</v>
@@ -6355,7 +6474,7 @@
         <v>9</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>9</v>
@@ -6370,7 +6489,7 @@
         <v>9</v>
       </c>
       <c r="G147" s="5" t="s">
-        <v>350</v>
+        <v>389</v>
       </c>
       <c r="H147" s="5" t="s">
         <v>9</v>
@@ -6387,13 +6506,13 @@
         <v>9</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>351</v>
+        <v>390</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>9</v>
@@ -6402,7 +6521,7 @@
         <v>9</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>352</v>
+        <v>391</v>
       </c>
       <c r="H148" s="3" t="s">
         <v>9</v>
@@ -6419,25 +6538,25 @@
         <v>9</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>353</v>
+        <v>392</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E149" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F149" s="4" t="s">
-        <v>354</v>
+        <v>393</v>
       </c>
       <c r="G149" s="5" t="s">
-        <v>355</v>
+        <v>394</v>
       </c>
       <c r="H149" s="5" t="s">
-        <v>356</v>
+        <v>395</v>
       </c>
       <c r="I149" s="5" t="s">
         <v>9</v>
@@ -6451,7 +6570,7 @@
         <v>9</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>357</v>
+        <v>396</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>9</v>
@@ -6466,7 +6585,7 @@
         <v>9</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>358</v>
+        <v>397</v>
       </c>
       <c r="H150" s="3" t="s">
         <v>9</v>
@@ -6483,22 +6602,22 @@
         <v>9</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>359</v>
+        <v>398</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E151" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>360</v>
+        <v>399</v>
       </c>
       <c r="G151" s="5" t="s">
-        <v>361</v>
+        <v>400</v>
       </c>
       <c r="H151" s="5" t="s">
         <v>9</v>
@@ -6515,7 +6634,7 @@
         <v>9</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>362</v>
+        <v>401</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>9</v>
@@ -6530,7 +6649,7 @@
         <v>9</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>363</v>
+        <v>402</v>
       </c>
       <c r="H152" s="3" t="s">
         <v>9</v>
@@ -6547,13 +6666,13 @@
         <v>9</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>364</v>
+        <v>403</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E153" s="4" t="s">
         <v>9</v>
@@ -6562,7 +6681,7 @@
         <v>9</v>
       </c>
       <c r="G153" s="5" t="s">
-        <v>365</v>
+        <v>404</v>
       </c>
       <c r="H153" s="5" t="s">
         <v>9</v>
@@ -6579,13 +6698,13 @@
         <v>9</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>366</v>
+        <v>405</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E154" s="2" t="s">
         <v>9</v>
@@ -6594,7 +6713,7 @@
         <v>9</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>367</v>
+        <v>406</v>
       </c>
       <c r="H154" s="3" t="s">
         <v>9</v>
@@ -6611,13 +6730,13 @@
         <v>9</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>368</v>
+        <v>407</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E155" s="4" t="s">
         <v>9</v>
@@ -6626,7 +6745,7 @@
         <v>9</v>
       </c>
       <c r="G155" s="5" t="s">
-        <v>369</v>
+        <v>408</v>
       </c>
       <c r="H155" s="5" t="s">
         <v>9</v>
@@ -6643,7 +6762,7 @@
         <v>9</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>370</v>
+        <v>409</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>9</v>
@@ -6658,7 +6777,7 @@
         <v>9</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>371</v>
+        <v>410</v>
       </c>
       <c r="H156" s="3" t="s">
         <v>9</v>
@@ -6675,7 +6794,7 @@
         <v>9</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>372</v>
+        <v>411</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>9</v>
@@ -6690,7 +6809,7 @@
         <v>9</v>
       </c>
       <c r="G157" s="5" t="s">
-        <v>373</v>
+        <v>412</v>
       </c>
       <c r="H157" s="5" t="s">
         <v>9</v>
@@ -6707,7 +6826,7 @@
         <v>9</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>374</v>
+        <v>413</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>9</v>
@@ -6722,7 +6841,7 @@
         <v>9</v>
       </c>
       <c r="G158" s="3" t="s">
-        <v>375</v>
+        <v>414</v>
       </c>
       <c r="H158" s="3" t="s">
         <v>9</v>
@@ -6739,13 +6858,13 @@
         <v>9</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>376</v>
+        <v>415</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E159" s="4" t="s">
         <v>9</v>
@@ -6754,10 +6873,10 @@
         <v>9</v>
       </c>
       <c r="G159" s="5" t="s">
-        <v>377</v>
+        <v>416</v>
       </c>
       <c r="H159" s="5" t="s">
-        <v>378</v>
+        <v>417</v>
       </c>
       <c r="I159" s="5" t="s">
         <v>9</v>
@@ -6771,13 +6890,13 @@
         <v>9</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>379</v>
+        <v>418</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>9</v>
@@ -6786,7 +6905,7 @@
         <v>9</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>380</v>
+        <v>419</v>
       </c>
       <c r="H160" s="3" t="s">
         <v>9</v>
@@ -6803,7 +6922,7 @@
         <v>9</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>381</v>
+        <v>420</v>
       </c>
       <c r="C161" s="4" t="s">
         <v>9</v>
@@ -6818,7 +6937,7 @@
         <v>9</v>
       </c>
       <c r="G161" s="5" t="s">
-        <v>382</v>
+        <v>421</v>
       </c>
       <c r="H161" s="5" t="s">
         <v>9</v>
@@ -6835,13 +6954,13 @@
         <v>9</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>383</v>
+        <v>422</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>9</v>
@@ -6850,7 +6969,7 @@
         <v>9</v>
       </c>
       <c r="G162" s="3" t="s">
-        <v>384</v>
+        <v>423</v>
       </c>
       <c r="H162" s="3" t="s">
         <v>9</v>
@@ -6867,13 +6986,13 @@
         <v>9</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>385</v>
+        <v>424</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E163" s="4" t="s">
         <v>9</v>
@@ -6882,7 +7001,7 @@
         <v>9</v>
       </c>
       <c r="G163" s="5" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="H163" s="5" t="s">
         <v>9</v>
@@ -6899,7 +7018,7 @@
         <v>9</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>387</v>
+        <v>426</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>9</v>
@@ -6914,7 +7033,7 @@
         <v>9</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>388</v>
+        <v>427</v>
       </c>
       <c r="H164" s="3" t="s">
         <v>9</v>
@@ -6931,7 +7050,7 @@
         <v>9</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>389</v>
+        <v>428</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>9</v>
@@ -6946,7 +7065,7 @@
         <v>9</v>
       </c>
       <c r="G165" s="5" t="s">
-        <v>390</v>
+        <v>429</v>
       </c>
       <c r="H165" s="5" t="s">
         <v>9</v>
@@ -6963,7 +7082,7 @@
         <v>9</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>391</v>
+        <v>430</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>9</v>
@@ -6978,7 +7097,7 @@
         <v>9</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>392</v>
+        <v>431</v>
       </c>
       <c r="H166" s="3" t="s">
         <v>9</v>
@@ -6995,13 +7114,13 @@
         <v>9</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>393</v>
+        <v>432</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E167" s="4" t="s">
         <v>9</v>
@@ -7010,7 +7129,7 @@
         <v>9</v>
       </c>
       <c r="G167" s="5" t="s">
-        <v>394</v>
+        <v>433</v>
       </c>
       <c r="H167" s="5" t="s">
         <v>9</v>
@@ -7027,7 +7146,7 @@
         <v>9</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>395</v>
+        <v>434</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>9</v>
@@ -7042,7 +7161,7 @@
         <v>9</v>
       </c>
       <c r="G168" s="3" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
       <c r="H168" s="3" t="s">
         <v>9</v>
@@ -7059,13 +7178,13 @@
         <v>9</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>397</v>
+        <v>436</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E169" s="4" t="s">
         <v>9</v>
@@ -7074,7 +7193,7 @@
         <v>9</v>
       </c>
       <c r="G169" s="5" t="s">
-        <v>380</v>
+        <v>419</v>
       </c>
       <c r="H169" s="5" t="s">
         <v>9</v>
@@ -7091,7 +7210,7 @@
         <v>9</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>9</v>
@@ -7103,10 +7222,10 @@
         <v>9</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
       <c r="G170" s="3" t="s">
-        <v>400</v>
+        <v>439</v>
       </c>
       <c r="H170" s="3" t="s">
         <v>9</v>
@@ -7123,7 +7242,7 @@
         <v>9</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>401</v>
+        <v>440</v>
       </c>
       <c r="C171" s="4" t="s">
         <v>9</v>
@@ -7135,10 +7254,10 @@
         <v>9</v>
       </c>
       <c r="F171" s="4" t="s">
-        <v>402</v>
+        <v>441</v>
       </c>
       <c r="G171" s="5" t="s">
-        <v>403</v>
+        <v>442</v>
       </c>
       <c r="H171" s="5" t="s">
         <v>9</v>
@@ -7155,7 +7274,7 @@
         <v>9</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>404</v>
+        <v>443</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>9</v>
@@ -7167,10 +7286,10 @@
         <v>9</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>405</v>
+        <v>444</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
       <c r="H172" s="3" t="s">
         <v>9</v>
@@ -7187,7 +7306,7 @@
         <v>9</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>407</v>
+        <v>446</v>
       </c>
       <c r="C173" s="4" t="s">
         <v>9</v>
@@ -7199,10 +7318,10 @@
         <v>9</v>
       </c>
       <c r="F173" s="4" t="s">
-        <v>408</v>
+        <v>447</v>
       </c>
       <c r="G173" s="5" t="s">
-        <v>409</v>
+        <v>448</v>
       </c>
       <c r="H173" s="5" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Fix 'boku' ruby text in S00032
</commit_message>
<xml_diff>
--- a/tl/S00032.MES.BIN.xlsx
+++ b/tl/S00032.MES.BIN.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F62336-5BE6-426D-9CD7-E172133199EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45D12C4-0F12-49ED-A013-83F2307AF3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="11190" windowWidth="45900" windowHeight="19845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="19755" windowWidth="54345" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00032.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -404,7 +404,7 @@
     <t>87</t>
   </si>
   <si>
-    <t>0</t>
+    <t>???</t>
   </si>
   <si>
     <t>…………</t>
@@ -842,7 +842,7 @@
     <t>193</t>
   </si>
   <si>
-    <t>Rina...Ogata-chan...</t>
+    <t>Ogata...Rina-chan...</t>
   </si>
   <si>
     <t>195</t>
@@ -872,7 +872,7 @@
     <t>203</t>
   </si>
   <si>
-    <t>In contrast to Yuki, who is naturally too relaxed and doesn’t have to worry about her private life, Rina's image is quite well-defined and it feels like her private life is always being watched.</t>
+    <t>In contrast to Yuki, who is naturally too relaxed and doesn't have to worry about her private life, Rina's image is quite well-defined and it feels like her private life is always being watched.</t>
   </si>
   <si>
     <t>Yuki is naturally too private and is not followed by the media, whereas her image is fairly solidified.</t>
@@ -1121,7 +1121,7 @@
     <t>265</t>
   </si>
   <si>
-    <t>Don't misunderstand me... I like &lt;Ryou|boku 僕&gt; the most you know, Rina-chan...</t>
+    <t>Don't misunderstand me... &lt;RI|boku 僕&gt; like you the most you know, Rina-chan...</t>
   </si>
   <si>
     <t>"Don't misunderstand me... I like you the most, Rina-chan..."</t>
@@ -1130,7 +1130,7 @@
     <t>267</t>
   </si>
   <si>
-    <t>Wh-what do you mean by "&lt;Ryou|boku 僕&gt;"? That's gross! And don't call me Rina-chan!</t>
+    <t>Wh-what do you mean by "&lt;RI|boku 僕&gt;"? That's gross! And don't call me Rina-chan!</t>
   </si>
   <si>
     <t>"Wh-what do you mean by 'I'?! That's disgusting!"</t>
@@ -1304,7 +1304,7 @@
     <t>317</t>
   </si>
   <si>
-    <t>Sorry, &lt;Rbud|君&gt;. I didn't think she's actually hit you.</t>
+    <t>Sorry, &lt;Rbud|君&gt;. I didn't think she'd actually hit you.</t>
   </si>
   <si>
     <t>Sorry, man... I didn't think she'd actually hit you...</t>
@@ -1840,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>